<commit_message>
Resultados de pruebas :/
</commit_message>
<xml_diff>
--- a/Results - Gustavo - 1010101010.xlsx
+++ b/Results - Gustavo - 1010101010.xlsx
@@ -4,13 +4,172 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="RRR" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>vanecan</author>
+  </authors>
+  <commentList>
+    <comment ref="A112" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>num_generations = 10000
+population_size = 500
+pool_size = 4
+const_max = 10.0
+step_size_const = 2
+p_reg_op2_const = 0.7
+p_const_in = 0.7
+p_macro_mutation = 0.45
+p_ins = 0.7
+p_del = 0.3
+p_micro_mutation = 0.95
+p_regmut = 0.5 
+p_opermut = 0.40
+p_constmut = 0.1
+p_crossover = 0.05</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A120" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>num_generations = 10000
+population_size = 500
+const_max = 25.0
+step_size_const = 2 
+p_reg_op2_const = 0.7
+p_const_in = 0.8
+p_macro_mutation = 0.6
+p_ins = 0.7 
+p_del = 0.3
+p_micro_mutation = 0.95
+p_regmut = 0.5 
+p_opermut = 0.40 
+p_constmut = 0.1 
+p_crossover = 0.05</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A122" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> num_generations = 10000
+ population_size = 500
+ pool_size = 4
+ const_max = 10.0
+ step_size_const = 0.5
+ p_reg_op2_const = 0.7
+ p_const_in = 0.7
+ p_macro_mutation = 0.4
+ p_ins = 0.7
+ p_del = 0.3
+ p_micro_mutation = 0.95
+ p_regmut = 0.5
+ p_opermut = 0.40
+ p_constmut = 0.1 
+ p_crossover = 0.2</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A124" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>num_generations = 10000
+population_size = 500
+pool_size = 4
+const_max = 5.0
+step_size_const = 2 
+p_reg_op2_const = 0.7
+p_const_in = 0.8
+p_macro_mutation = 0.6
+p_ins = 0.7
+p_del = 0.3
+p_micro_mutation = 0.95
+p_regmut = 0.5
+p_opermut = 0.40
+p_constmut = 0.1 
+p_crossover = 0.05</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A126" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>num_generations = 10000
+population_size = 500
+pool_size = 4
+const_max = 10.0
+step_size_const = 0.5
+p_reg_op2_const = 0.7
+p_const_in = 0.7
+p_macro_mutation = 0.4
+p_ins = 0.7
+p_del = 0.3
+p_micro_mutation = 0.95
+p_regmut = 0.5
+p_opermut = 0.40
+p_constmut = 0.1 
+p_crossover = 0.05</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26,7 +185,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,8 +321,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,12 +523,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -369,12 +535,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -635,19 +837,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -726,6 +915,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -771,35 +1019,99 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="41" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1141,11 +1453,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U107"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A107" sqref="A1:XFD107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,7 +1467,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="14">
+      <c r="B1" s="13">
         <v>1</v>
       </c>
       <c r="C1" s="4">
@@ -1220,7 +1532,7 @@
       <c r="A2" s="7">
         <v>144</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14">
         <v>21.468403494018901</v>
       </c>
       <c r="C2" s="3">
@@ -1277,7 +1589,7 @@
       <c r="T2" s="3">
         <v>122.974149078835</v>
       </c>
-      <c r="U2" s="16">
+      <c r="U2" s="15">
         <v>18.832553116792202</v>
       </c>
     </row>
@@ -1285,7 +1597,7 @@
       <c r="A3" s="8">
         <v>145</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="16">
         <v>30.621474445603099</v>
       </c>
       <c r="C3" s="1">
@@ -1342,7 +1654,7 @@
       <c r="T3" s="1">
         <v>52.823391488371698</v>
       </c>
-      <c r="U3" s="18">
+      <c r="U3" s="17">
         <v>66.801683974615798</v>
       </c>
     </row>
@@ -1350,7 +1662,7 @@
       <c r="A4" s="8">
         <v>146</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>1.5929773377246701</v>
       </c>
       <c r="C4" s="1">
@@ -1407,7 +1719,7 @@
       <c r="T4" s="1">
         <v>256.26530248787202</v>
       </c>
-      <c r="U4" s="18">
+      <c r="U4" s="17">
         <v>0.412204063045151</v>
       </c>
     </row>
@@ -1415,7 +1727,7 @@
       <c r="A5" s="8">
         <v>147</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="16">
         <v>11.9480417717726</v>
       </c>
       <c r="C5" s="1">
@@ -1472,7 +1784,7 @@
       <c r="T5" s="1">
         <v>15.3769698195636</v>
       </c>
-      <c r="U5" s="18">
+      <c r="U5" s="17">
         <v>0.14802647062111901</v>
       </c>
     </row>
@@ -1480,7 +1792,7 @@
       <c r="A6" s="8">
         <v>148</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>106.882758808185</v>
       </c>
       <c r="C6" s="1">
@@ -1537,7 +1849,7 @@
       <c r="T6" s="1">
         <v>46.142908673837397</v>
       </c>
-      <c r="U6" s="18">
+      <c r="U6" s="17">
         <v>4.2825350969779201</v>
       </c>
     </row>
@@ -1545,7 +1857,7 @@
       <c r="A7" s="8">
         <v>149</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>15.5810151059757</v>
       </c>
       <c r="C7" s="1">
@@ -1602,7 +1914,7 @@
       <c r="T7" s="1">
         <v>138.926698206184</v>
       </c>
-      <c r="U7" s="18">
+      <c r="U7" s="17">
         <v>207.370382741116</v>
       </c>
     </row>
@@ -1610,7 +1922,7 @@
       <c r="A8" s="8">
         <v>150</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="16">
         <v>37.386624069382002</v>
       </c>
       <c r="C8" s="1">
@@ -1667,7 +1979,7 @@
       <c r="T8" s="1">
         <v>2.3206119491300901</v>
       </c>
-      <c r="U8" s="18">
+      <c r="U8" s="17">
         <v>82.134655714920797</v>
       </c>
     </row>
@@ -1675,7 +1987,7 @@
       <c r="A9" s="8">
         <v>151</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>29.135478942174601</v>
       </c>
       <c r="C9" s="1">
@@ -1732,7 +2044,7 @@
       <c r="T9" s="1">
         <v>15.8860384616444</v>
       </c>
-      <c r="U9" s="18">
+      <c r="U9" s="17">
         <v>8.9899446694007192</v>
       </c>
     </row>
@@ -1740,7 +2052,7 @@
       <c r="A10" s="8">
         <v>152</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="16">
         <v>7.2095363708380598E-3</v>
       </c>
       <c r="C10" s="1">
@@ -1797,7 +2109,7 @@
       <c r="T10" s="1">
         <v>1.28521546362743</v>
       </c>
-      <c r="U10" s="18">
+      <c r="U10" s="17">
         <v>5.2497741289216604</v>
       </c>
     </row>
@@ -1805,7 +2117,7 @@
       <c r="A11" s="8">
         <v>153</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>19.849076373651201</v>
       </c>
       <c r="C11" s="1">
@@ -1862,7 +2174,7 @@
       <c r="T11" s="1">
         <v>22.188168684704898</v>
       </c>
-      <c r="U11" s="18">
+      <c r="U11" s="17">
         <v>1.94586550165712</v>
       </c>
     </row>
@@ -1870,7 +2182,7 @@
       <c r="A12" s="8">
         <v>154</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>1.85706346049278</v>
       </c>
       <c r="C12" s="1">
@@ -1927,7 +2239,7 @@
       <c r="T12" s="1">
         <v>38.807940921105804</v>
       </c>
-      <c r="U12" s="18">
+      <c r="U12" s="17">
         <v>0.44229397942567</v>
       </c>
     </row>
@@ -1935,7 +2247,7 @@
       <c r="A13" s="8">
         <v>155</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="16">
         <v>5.0563305451335196</v>
       </c>
       <c r="C13" s="1">
@@ -1992,7 +2304,7 @@
       <c r="T13" s="1">
         <v>0.98647139664379402</v>
       </c>
-      <c r="U13" s="18">
+      <c r="U13" s="17">
         <v>15.4046837816067</v>
       </c>
     </row>
@@ -2000,7 +2312,7 @@
       <c r="A14" s="8">
         <v>156</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="16">
         <v>2.7632499087792199</v>
       </c>
       <c r="C14" s="1">
@@ -2057,7 +2369,7 @@
       <c r="T14" s="1">
         <v>68.102185567857902</v>
       </c>
-      <c r="U14" s="18">
+      <c r="U14" s="17">
         <v>8.9533046928742301</v>
       </c>
     </row>
@@ -2065,7 +2377,7 @@
       <c r="A15" s="8">
         <v>157</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="16">
         <v>27.747334148459199</v>
       </c>
       <c r="C15" s="1">
@@ -2122,7 +2434,7 @@
       <c r="T15" s="1">
         <v>1.55767506298028</v>
       </c>
-      <c r="U15" s="18">
+      <c r="U15" s="17">
         <v>60.366556116807203</v>
       </c>
     </row>
@@ -2130,7 +2442,7 @@
       <c r="A16" s="8">
         <v>158</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="16">
         <v>254.16786565579599</v>
       </c>
       <c r="C16" s="1">
@@ -2187,7 +2499,7 @@
       <c r="T16" s="1">
         <v>9.9518333060017294</v>
       </c>
-      <c r="U16" s="18">
+      <c r="U16" s="17">
         <v>1.4154755195534401</v>
       </c>
     </row>
@@ -2195,7 +2507,7 @@
       <c r="A17" s="8">
         <v>159</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="16">
         <v>137.15898473867099</v>
       </c>
       <c r="C17" s="1">
@@ -2252,7 +2564,7 @@
       <c r="T17" s="1">
         <v>0.84890704532888495</v>
       </c>
-      <c r="U17" s="18">
+      <c r="U17" s="17">
         <v>8.3762370728515407E-3</v>
       </c>
     </row>
@@ -2260,7 +2572,7 @@
       <c r="A18" s="8">
         <v>160</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="16">
         <v>47.566716209700203</v>
       </c>
       <c r="C18" s="1">
@@ -2317,7 +2629,7 @@
       <c r="T18" s="1">
         <v>217.32540233068099</v>
       </c>
-      <c r="U18" s="18">
+      <c r="U18" s="17">
         <v>23.445475770823101</v>
       </c>
     </row>
@@ -2325,7 +2637,7 @@
       <c r="A19" s="8">
         <v>161</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="16">
         <v>313.49625264576099</v>
       </c>
       <c r="C19" s="1">
@@ -2382,7 +2694,7 @@
       <c r="T19" s="1">
         <v>4.5795257789600896</v>
       </c>
-      <c r="U19" s="18">
+      <c r="U19" s="17">
         <v>16.2067224727862</v>
       </c>
     </row>
@@ -2390,7 +2702,7 @@
       <c r="A20" s="8">
         <v>162</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="16">
         <v>145.70728520075099</v>
       </c>
       <c r="C20" s="1">
@@ -2447,7 +2759,7 @@
       <c r="T20" s="1">
         <v>170.10642944965801</v>
       </c>
-      <c r="U20" s="18">
+      <c r="U20" s="17">
         <v>170.39420035504801</v>
       </c>
     </row>
@@ -2455,7 +2767,7 @@
       <c r="A21" s="8">
         <v>163</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="16">
         <v>41.384606431698998</v>
       </c>
       <c r="C21" s="2">
@@ -2512,7 +2824,7 @@
       <c r="T21" s="1">
         <v>758.62577903299098</v>
       </c>
-      <c r="U21" s="18">
+      <c r="U21" s="17">
         <v>5.6554113715091301</v>
       </c>
     </row>
@@ -2520,7 +2832,7 @@
       <c r="A22" s="8">
         <v>164</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="16">
         <v>581.97887697430201</v>
       </c>
       <c r="C22" s="1">
@@ -2577,7 +2889,7 @@
       <c r="T22" s="1">
         <v>42.214175190134398</v>
       </c>
-      <c r="U22" s="19">
+      <c r="U22" s="18">
         <v>1.2016802140640201E-5</v>
       </c>
     </row>
@@ -2585,7 +2897,7 @@
       <c r="A23" s="8">
         <v>165</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="16">
         <v>117.489151794066</v>
       </c>
       <c r="C23" s="1">
@@ -2642,7 +2954,7 @@
       <c r="T23" s="1">
         <v>155.23383950477299</v>
       </c>
-      <c r="U23" s="18">
+      <c r="U23" s="17">
         <v>44.509751461826298</v>
       </c>
     </row>
@@ -2650,7 +2962,7 @@
       <c r="A24" s="8">
         <v>166</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="16">
         <v>88.531521544392902</v>
       </c>
       <c r="C24" s="1">
@@ -2707,7 +3019,7 @@
       <c r="T24" s="1">
         <v>40.148737497934</v>
       </c>
-      <c r="U24" s="18">
+      <c r="U24" s="17">
         <v>112.56814649866</v>
       </c>
     </row>
@@ -2715,7 +3027,7 @@
       <c r="A25" s="8">
         <v>167</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="16">
         <v>10.063841855633701</v>
       </c>
       <c r="C25" s="1">
@@ -2772,7 +3084,7 @@
       <c r="T25" s="1">
         <v>16.643191848894599</v>
       </c>
-      <c r="U25" s="18">
+      <c r="U25" s="17">
         <v>145.51150690750799</v>
       </c>
     </row>
@@ -2780,7 +3092,7 @@
       <c r="A26" s="8">
         <v>168</v>
       </c>
-      <c r="B26" s="17">
+      <c r="B26" s="16">
         <v>16.669373770350301</v>
       </c>
       <c r="C26" s="1">
@@ -2837,7 +3149,7 @@
       <c r="T26" s="1">
         <v>57.998591627398099</v>
       </c>
-      <c r="U26" s="18">
+      <c r="U26" s="17">
         <v>42.748456282381397</v>
       </c>
     </row>
@@ -2845,7 +3157,7 @@
       <c r="A27" s="8">
         <v>169</v>
       </c>
-      <c r="B27" s="17">
+      <c r="B27" s="16">
         <v>35.933421702320501</v>
       </c>
       <c r="C27" s="1">
@@ -2902,7 +3214,7 @@
       <c r="T27" s="1">
         <v>0.151932091547475</v>
       </c>
-      <c r="U27" s="18">
+      <c r="U27" s="17">
         <v>2.3899826409584901</v>
       </c>
     </row>
@@ -2910,7 +3222,7 @@
       <c r="A28" s="8">
         <v>170</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="16">
         <v>84.200874843417694</v>
       </c>
       <c r="C28" s="1">
@@ -2967,7 +3279,7 @@
       <c r="T28" s="1">
         <v>241.394670162344</v>
       </c>
-      <c r="U28" s="18">
+      <c r="U28" s="17">
         <v>6.8815514754952803E-2</v>
       </c>
     </row>
@@ -2975,7 +3287,7 @@
       <c r="A29" s="8">
         <v>171</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="16">
         <v>237.80070089344201</v>
       </c>
       <c r="C29" s="1">
@@ -3032,7 +3344,7 @@
       <c r="T29" s="1">
         <v>219.76958913016199</v>
       </c>
-      <c r="U29" s="18">
+      <c r="U29" s="17">
         <v>37.340095628323198</v>
       </c>
     </row>
@@ -3040,7 +3352,7 @@
       <c r="A30" s="8">
         <v>172</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="16">
         <v>379.48605407182998</v>
       </c>
       <c r="C30" s="1">
@@ -3097,7 +3409,7 @@
       <c r="T30" s="1">
         <v>586.63887522236905</v>
       </c>
-      <c r="U30" s="18">
+      <c r="U30" s="17">
         <v>33.027146264657397</v>
       </c>
     </row>
@@ -3105,7 +3417,7 @@
       <c r="A31" s="8">
         <v>173</v>
       </c>
-      <c r="B31" s="17">
+      <c r="B31" s="16">
         <v>60.232342852935801</v>
       </c>
       <c r="C31" s="1">
@@ -3162,7 +3474,7 @@
       <c r="T31" s="1">
         <v>185.44950494372301</v>
       </c>
-      <c r="U31" s="18">
+      <c r="U31" s="17">
         <v>925.21845589971201</v>
       </c>
     </row>
@@ -3170,7 +3482,7 @@
       <c r="A32" s="8">
         <v>174</v>
       </c>
-      <c r="B32" s="17">
+      <c r="B32" s="16">
         <v>111.05763228253799</v>
       </c>
       <c r="C32" s="1">
@@ -3227,7 +3539,7 @@
       <c r="T32" s="1">
         <v>1056.5955160937999</v>
       </c>
-      <c r="U32" s="18">
+      <c r="U32" s="17">
         <v>330.08077997817003</v>
       </c>
     </row>
@@ -3235,7 +3547,7 @@
       <c r="A33" s="8">
         <v>175</v>
       </c>
-      <c r="B33" s="17">
+      <c r="B33" s="16">
         <v>225.49497975204099</v>
       </c>
       <c r="C33" s="1">
@@ -3292,7 +3604,7 @@
       <c r="T33" s="1">
         <v>90.459727507147306</v>
       </c>
-      <c r="U33" s="18">
+      <c r="U33" s="17">
         <v>150.00506632117899</v>
       </c>
     </row>
@@ -3300,7 +3612,7 @@
       <c r="A34" s="8">
         <v>176</v>
       </c>
-      <c r="B34" s="17">
+      <c r="B34" s="16">
         <v>409.427888562367</v>
       </c>
       <c r="C34" s="1">
@@ -3357,7 +3669,7 @@
       <c r="T34" s="1">
         <v>58.2003220511519</v>
       </c>
-      <c r="U34" s="18">
+      <c r="U34" s="17">
         <v>22.602483075808198</v>
       </c>
     </row>
@@ -3365,7 +3677,7 @@
       <c r="A35" s="8">
         <v>177</v>
       </c>
-      <c r="B35" s="17">
+      <c r="B35" s="16">
         <v>164.14442234982999</v>
       </c>
       <c r="C35" s="1">
@@ -3422,7 +3734,7 @@
       <c r="T35" s="1">
         <v>46.872934496324902</v>
       </c>
-      <c r="U35" s="18">
+      <c r="U35" s="17">
         <v>299.13416121133702</v>
       </c>
     </row>
@@ -3430,7 +3742,7 @@
       <c r="A36" s="8">
         <v>178</v>
       </c>
-      <c r="B36" s="17">
+      <c r="B36" s="16">
         <v>53.869356435240803</v>
       </c>
       <c r="C36" s="1">
@@ -3487,7 +3799,7 @@
       <c r="T36" s="1">
         <v>356.70683461573998</v>
       </c>
-      <c r="U36" s="18">
+      <c r="U36" s="17">
         <v>284.84616150795603</v>
       </c>
     </row>
@@ -3495,7 +3807,7 @@
       <c r="A37" s="8">
         <v>179</v>
       </c>
-      <c r="B37" s="17">
+      <c r="B37" s="16">
         <v>34.650742342693597</v>
       </c>
       <c r="C37" s="1">
@@ -3552,7 +3864,7 @@
       <c r="T37" s="1">
         <v>657.81074119787002</v>
       </c>
-      <c r="U37" s="18">
+      <c r="U37" s="17">
         <v>270.06709990417602</v>
       </c>
     </row>
@@ -3560,7 +3872,7 @@
       <c r="A38" s="8">
         <v>180</v>
       </c>
-      <c r="B38" s="17">
+      <c r="B38" s="16">
         <v>146.61351139565801</v>
       </c>
       <c r="C38" s="1">
@@ -3617,7 +3929,7 @@
       <c r="T38" s="1">
         <v>378.32526593877498</v>
       </c>
-      <c r="U38" s="18">
+      <c r="U38" s="17">
         <v>273.36342616621903</v>
       </c>
     </row>
@@ -3625,7 +3937,7 @@
       <c r="A39" s="8">
         <v>181</v>
       </c>
-      <c r="B39" s="17">
+      <c r="B39" s="16">
         <v>111.25458000453899</v>
       </c>
       <c r="C39" s="1">
@@ -3682,7 +3994,7 @@
       <c r="T39" s="1">
         <v>7.6907779583400799</v>
       </c>
-      <c r="U39" s="18">
+      <c r="U39" s="17">
         <v>452.09946477438098</v>
       </c>
     </row>
@@ -3690,7 +4002,7 @@
       <c r="A40" s="8">
         <v>182</v>
       </c>
-      <c r="B40" s="17">
+      <c r="B40" s="16">
         <v>120.807825308817</v>
       </c>
       <c r="C40" s="1">
@@ -3747,7 +4059,7 @@
       <c r="T40" s="1">
         <v>201.882022175879</v>
       </c>
-      <c r="U40" s="18">
+      <c r="U40" s="17">
         <v>257.45543181158001</v>
       </c>
     </row>
@@ -3755,7 +4067,7 @@
       <c r="A41" s="8">
         <v>183</v>
       </c>
-      <c r="B41" s="17">
+      <c r="B41" s="16">
         <v>553.554261399604</v>
       </c>
       <c r="C41" s="1">
@@ -3812,7 +4124,7 @@
       <c r="T41" s="1">
         <v>177.74827054257599</v>
       </c>
-      <c r="U41" s="18">
+      <c r="U41" s="17">
         <v>705.71500260275104</v>
       </c>
     </row>
@@ -3820,7 +4132,7 @@
       <c r="A42" s="8">
         <v>184</v>
       </c>
-      <c r="B42" s="17">
+      <c r="B42" s="16">
         <v>79.193458627955906</v>
       </c>
       <c r="C42" s="1">
@@ -3877,7 +4189,7 @@
       <c r="T42" s="1">
         <v>303.778884432604</v>
       </c>
-      <c r="U42" s="18">
+      <c r="U42" s="17">
         <v>545.45820736786197</v>
       </c>
     </row>
@@ -3885,7 +4197,7 @@
       <c r="A43" s="8">
         <v>185</v>
       </c>
-      <c r="B43" s="17">
+      <c r="B43" s="16">
         <v>606.53783934908097</v>
       </c>
       <c r="C43" s="1">
@@ -3942,7 +4254,7 @@
       <c r="T43" s="1">
         <v>59.463187077149797</v>
       </c>
-      <c r="U43" s="18">
+      <c r="U43" s="17">
         <v>991.56610110738302</v>
       </c>
     </row>
@@ -3950,7 +4262,7 @@
       <c r="A44" s="8">
         <v>186</v>
       </c>
-      <c r="B44" s="17">
+      <c r="B44" s="16">
         <v>143.687915100374</v>
       </c>
       <c r="C44" s="1">
@@ -4007,7 +4319,7 @@
       <c r="T44" s="1">
         <v>2.0285637497630802</v>
       </c>
-      <c r="U44" s="18">
+      <c r="U44" s="17">
         <v>1127.2941332509499</v>
       </c>
     </row>
@@ -4015,7 +4327,7 @@
       <c r="A45" s="8">
         <v>187</v>
       </c>
-      <c r="B45" s="17">
+      <c r="B45" s="16">
         <v>206.74614782541099</v>
       </c>
       <c r="C45" s="1">
@@ -4072,7 +4384,7 @@
       <c r="T45" s="1">
         <v>35.456631505136997</v>
       </c>
-      <c r="U45" s="18">
+      <c r="U45" s="17">
         <v>526.16330779288296</v>
       </c>
     </row>
@@ -4080,7 +4392,7 @@
       <c r="A46" s="8">
         <v>188</v>
       </c>
-      <c r="B46" s="17">
+      <c r="B46" s="16">
         <v>192.509997132526</v>
       </c>
       <c r="C46" s="1">
@@ -4137,7 +4449,7 @@
       <c r="T46" s="1">
         <v>16.823790044384499</v>
       </c>
-      <c r="U46" s="18">
+      <c r="U46" s="17">
         <v>380.39405017617298</v>
       </c>
     </row>
@@ -4145,7 +4457,7 @@
       <c r="A47" s="8">
         <v>189</v>
       </c>
-      <c r="B47" s="17">
+      <c r="B47" s="16">
         <v>140.13468462280201</v>
       </c>
       <c r="C47" s="1">
@@ -4202,7 +4514,7 @@
       <c r="T47" s="1">
         <v>45.916005360066102</v>
       </c>
-      <c r="U47" s="18">
+      <c r="U47" s="17">
         <v>1535.9267208839899</v>
       </c>
     </row>
@@ -4210,7 +4522,7 @@
       <c r="A48" s="8">
         <v>190</v>
       </c>
-      <c r="B48" s="17">
+      <c r="B48" s="16">
         <v>66.391325516333495</v>
       </c>
       <c r="C48" s="1">
@@ -4267,7 +4579,7 @@
       <c r="T48" s="1">
         <v>1.1012389917149201E-3</v>
       </c>
-      <c r="U48" s="18">
+      <c r="U48" s="17">
         <v>1597.71429281732</v>
       </c>
     </row>
@@ -4275,7 +4587,7 @@
       <c r="A49" s="8">
         <v>191</v>
       </c>
-      <c r="B49" s="17">
+      <c r="B49" s="16">
         <v>219.87777084738099</v>
       </c>
       <c r="C49" s="1">
@@ -4332,7 +4644,7 @@
       <c r="T49" s="1">
         <v>44.8556395836831</v>
       </c>
-      <c r="U49" s="18">
+      <c r="U49" s="17">
         <v>1195.0624372171401</v>
       </c>
     </row>
@@ -4340,7 +4652,7 @@
       <c r="A50" s="8">
         <v>192</v>
       </c>
-      <c r="B50" s="17">
+      <c r="B50" s="16">
         <v>458.64367072115499</v>
       </c>
       <c r="C50" s="1">
@@ -4397,7 +4709,7 @@
       <c r="T50" s="1">
         <v>216.162545795146</v>
       </c>
-      <c r="U50" s="18">
+      <c r="U50" s="17">
         <v>834.49955926788402</v>
       </c>
     </row>
@@ -4405,7 +4717,7 @@
       <c r="A51" s="8">
         <v>193</v>
       </c>
-      <c r="B51" s="17">
+      <c r="B51" s="16">
         <v>135.961042646609</v>
       </c>
       <c r="C51" s="1">
@@ -4462,7 +4774,7 @@
       <c r="T51" s="1">
         <v>2.8768820439046299</v>
       </c>
-      <c r="U51" s="18">
+      <c r="U51" s="17">
         <v>590.02262068324205</v>
       </c>
     </row>
@@ -4470,7 +4782,7 @@
       <c r="A52" s="8">
         <v>194</v>
       </c>
-      <c r="B52" s="17">
+      <c r="B52" s="16">
         <v>876.08342898460603</v>
       </c>
       <c r="C52" s="1">
@@ -4527,7 +4839,7 @@
       <c r="T52" s="1">
         <v>5.9472010786340403</v>
       </c>
-      <c r="U52" s="18">
+      <c r="U52" s="17">
         <v>665.40927767419703</v>
       </c>
     </row>
@@ -4535,7 +4847,7 @@
       <c r="A53" s="8">
         <v>195</v>
       </c>
-      <c r="B53" s="17">
+      <c r="B53" s="16">
         <v>706.79288394725097</v>
       </c>
       <c r="C53" s="1">
@@ -4592,7 +4904,7 @@
       <c r="T53" s="1">
         <v>69.912906019100902</v>
       </c>
-      <c r="U53" s="18">
+      <c r="U53" s="17">
         <v>611.61139749755796</v>
       </c>
     </row>
@@ -4600,7 +4912,7 @@
       <c r="A54" s="8">
         <v>196</v>
       </c>
-      <c r="B54" s="17">
+      <c r="B54" s="16">
         <v>146.82385576476301</v>
       </c>
       <c r="C54" s="1">
@@ -4657,7 +4969,7 @@
       <c r="T54" s="1">
         <v>22.9959536945486</v>
       </c>
-      <c r="U54" s="18">
+      <c r="U54" s="17">
         <v>732.68075437208495</v>
       </c>
     </row>
@@ -4665,7 +4977,7 @@
       <c r="A55" s="8">
         <v>197</v>
       </c>
-      <c r="B55" s="17">
+      <c r="B55" s="16">
         <v>256.529286321342</v>
       </c>
       <c r="C55" s="1">
@@ -4722,7 +5034,7 @@
       <c r="T55" s="1">
         <v>316.578912105526</v>
       </c>
-      <c r="U55" s="18">
+      <c r="U55" s="17">
         <v>1410.4017930703001</v>
       </c>
     </row>
@@ -4730,7 +5042,7 @@
       <c r="A56" s="8">
         <v>198</v>
       </c>
-      <c r="B56" s="17">
+      <c r="B56" s="16">
         <v>512.33660062065201</v>
       </c>
       <c r="C56" s="1">
@@ -4787,7 +5099,7 @@
       <c r="T56" s="1">
         <v>47.782765332735899</v>
       </c>
-      <c r="U56" s="18">
+      <c r="U56" s="17">
         <v>468.03718900975099</v>
       </c>
     </row>
@@ -4795,7 +5107,7 @@
       <c r="A57" s="8">
         <v>199</v>
       </c>
-      <c r="B57" s="17">
+      <c r="B57" s="16">
         <v>115.893836750322</v>
       </c>
       <c r="C57" s="1">
@@ -4852,7 +5164,7 @@
       <c r="T57" s="1">
         <v>106.35248847724201</v>
       </c>
-      <c r="U57" s="18">
+      <c r="U57" s="17">
         <v>528.46309888795804</v>
       </c>
     </row>
@@ -4860,7 +5172,7 @@
       <c r="A58" s="8">
         <v>200</v>
       </c>
-      <c r="B58" s="17">
+      <c r="B58" s="16">
         <v>90.503403864646899</v>
       </c>
       <c r="C58" s="1">
@@ -4917,7 +5229,7 @@
       <c r="T58" s="1">
         <v>10.4236083908821</v>
       </c>
-      <c r="U58" s="18">
+      <c r="U58" s="17">
         <v>1432.28940448769</v>
       </c>
     </row>
@@ -4925,7 +5237,7 @@
       <c r="A59" s="8">
         <v>201</v>
       </c>
-      <c r="B59" s="17">
+      <c r="B59" s="16">
         <v>409.20323147176202</v>
       </c>
       <c r="C59" s="1">
@@ -4982,7 +5294,7 @@
       <c r="T59" s="1">
         <v>3.6328557081298598</v>
       </c>
-      <c r="U59" s="18">
+      <c r="U59" s="17">
         <v>819.67233489287696</v>
       </c>
     </row>
@@ -4990,7 +5302,7 @@
       <c r="A60" s="8">
         <v>202</v>
       </c>
-      <c r="B60" s="17">
+      <c r="B60" s="16">
         <v>250.11789686444899</v>
       </c>
       <c r="C60" s="1">
@@ -5047,7 +5359,7 @@
       <c r="T60" s="1">
         <v>12.218040300307701</v>
       </c>
-      <c r="U60" s="18">
+      <c r="U60" s="17">
         <v>889.63936951124197</v>
       </c>
     </row>
@@ -5055,7 +5367,7 @@
       <c r="A61" s="8">
         <v>203</v>
       </c>
-      <c r="B61" s="17">
+      <c r="B61" s="16">
         <v>379.91260167840898</v>
       </c>
       <c r="C61" s="1">
@@ -5112,7 +5424,7 @@
       <c r="T61" s="1">
         <v>182.713585574289</v>
       </c>
-      <c r="U61" s="18">
+      <c r="U61" s="17">
         <v>182.65279057514499</v>
       </c>
     </row>
@@ -5120,7 +5432,7 @@
       <c r="A62" s="8">
         <v>204</v>
       </c>
-      <c r="B62" s="17">
+      <c r="B62" s="16">
         <v>158.69319663688299</v>
       </c>
       <c r="C62" s="1">
@@ -5177,7 +5489,7 @@
       <c r="T62" s="1">
         <v>4.6242074076275097</v>
       </c>
-      <c r="U62" s="18">
+      <c r="U62" s="17">
         <v>164.75699604967599</v>
       </c>
     </row>
@@ -5185,7 +5497,7 @@
       <c r="A63" s="8">
         <v>205</v>
       </c>
-      <c r="B63" s="17">
+      <c r="B63" s="16">
         <v>132.31813434068999</v>
       </c>
       <c r="C63" s="1">
@@ -5242,7 +5554,7 @@
       <c r="T63" s="1">
         <v>5.4772229785519997</v>
       </c>
-      <c r="U63" s="18">
+      <c r="U63" s="17">
         <v>184.79997090204799</v>
       </c>
     </row>
@@ -5250,7 +5562,7 @@
       <c r="A64" s="8">
         <v>206</v>
       </c>
-      <c r="B64" s="17">
+      <c r="B64" s="16">
         <v>411.87780426759201</v>
       </c>
       <c r="C64" s="1">
@@ -5307,7 +5619,7 @@
       <c r="T64" s="1">
         <v>19.3466352313817</v>
       </c>
-      <c r="U64" s="18">
+      <c r="U64" s="17">
         <v>3.9368837579132601</v>
       </c>
     </row>
@@ -5315,7 +5627,7 @@
       <c r="A65" s="8">
         <v>207</v>
       </c>
-      <c r="B65" s="17">
+      <c r="B65" s="16">
         <v>170.93400495750299</v>
       </c>
       <c r="C65" s="1">
@@ -5372,7 +5684,7 @@
       <c r="T65" s="1">
         <v>82.285499245175799</v>
       </c>
-      <c r="U65" s="18">
+      <c r="U65" s="17">
         <v>5.8482066818468299</v>
       </c>
     </row>
@@ -5380,7 +5692,7 @@
       <c r="A66" s="8">
         <v>208</v>
       </c>
-      <c r="B66" s="17">
+      <c r="B66" s="16">
         <v>273.908225022078</v>
       </c>
       <c r="C66" s="1">
@@ -5437,7 +5749,7 @@
       <c r="T66" s="1">
         <v>10.203483858574099</v>
       </c>
-      <c r="U66" s="18">
+      <c r="U66" s="17">
         <v>61.537427137248002</v>
       </c>
     </row>
@@ -5445,7 +5757,7 @@
       <c r="A67" s="8">
         <v>209</v>
       </c>
-      <c r="B67" s="17">
+      <c r="B67" s="16">
         <v>7.2737883074081404</v>
       </c>
       <c r="C67" s="1">
@@ -5502,7 +5814,7 @@
       <c r="T67" s="1">
         <v>2.22173174408191</v>
       </c>
-      <c r="U67" s="18">
+      <c r="U67" s="17">
         <v>133.56108922537001</v>
       </c>
     </row>
@@ -5510,7 +5822,7 @@
       <c r="A68" s="8">
         <v>210</v>
       </c>
-      <c r="B68" s="17">
+      <c r="B68" s="16">
         <v>108.252654248734</v>
       </c>
       <c r="C68" s="1">
@@ -5567,7 +5879,7 @@
       <c r="T68" s="1">
         <v>30.5063875477938</v>
       </c>
-      <c r="U68" s="18">
+      <c r="U68" s="17">
         <v>7.6749342933265297E-2</v>
       </c>
     </row>
@@ -5575,7 +5887,7 @@
       <c r="A69" s="8">
         <v>211</v>
       </c>
-      <c r="B69" s="17">
+      <c r="B69" s="16">
         <v>1112.3429767371399</v>
       </c>
       <c r="C69" s="1">
@@ -5632,7 +5944,7 @@
       <c r="T69" s="1">
         <v>367.47994785466699</v>
       </c>
-      <c r="U69" s="18">
+      <c r="U69" s="17">
         <v>117.863826836109</v>
       </c>
     </row>
@@ -5640,7 +5952,7 @@
       <c r="A70" s="8">
         <v>212</v>
       </c>
-      <c r="B70" s="17">
+      <c r="B70" s="16">
         <v>970.26732776182496</v>
       </c>
       <c r="C70" s="1">
@@ -5697,7 +6009,7 @@
       <c r="T70" s="1">
         <v>53.948771496184598</v>
       </c>
-      <c r="U70" s="18">
+      <c r="U70" s="17">
         <v>0.18207338411521901</v>
       </c>
     </row>
@@ -5705,7 +6017,7 @@
       <c r="A71" s="8">
         <v>213</v>
       </c>
-      <c r="B71" s="17">
+      <c r="B71" s="16">
         <v>555.79986479160004</v>
       </c>
       <c r="C71" s="1">
@@ -5762,7 +6074,7 @@
       <c r="T71" s="1">
         <v>1.35082331216443</v>
       </c>
-      <c r="U71" s="18">
+      <c r="U71" s="17">
         <v>12.770629849637199</v>
       </c>
     </row>
@@ -5770,7 +6082,7 @@
       <c r="A72" s="8">
         <v>214</v>
       </c>
-      <c r="B72" s="17">
+      <c r="B72" s="16">
         <v>178.33692308447701</v>
       </c>
       <c r="C72" s="1">
@@ -5827,7 +6139,7 @@
       <c r="T72" s="1">
         <v>23.487445891723599</v>
       </c>
-      <c r="U72" s="18">
+      <c r="U72" s="17">
         <v>15.759718924532599</v>
       </c>
     </row>
@@ -5835,7 +6147,7 @@
       <c r="A73" s="8">
         <v>215</v>
       </c>
-      <c r="B73" s="17">
+      <c r="B73" s="16">
         <v>38.998221785043199</v>
       </c>
       <c r="C73" s="1">
@@ -5892,7 +6204,7 @@
       <c r="T73" s="1">
         <v>5.0326187565348501</v>
       </c>
-      <c r="U73" s="18">
+      <c r="U73" s="17">
         <v>29.446963365578501</v>
       </c>
     </row>
@@ -5900,7 +6212,7 @@
       <c r="A74" s="8">
         <v>216</v>
       </c>
-      <c r="B74" s="17">
+      <c r="B74" s="16">
         <v>9.4297053517937304</v>
       </c>
       <c r="C74" s="1">
@@ -5957,7 +6269,7 @@
       <c r="T74" s="1">
         <v>28.970024446171301</v>
       </c>
-      <c r="U74" s="18">
+      <c r="U74" s="17">
         <v>14.531676679255099</v>
       </c>
     </row>
@@ -5965,7 +6277,7 @@
       <c r="A75" s="8">
         <v>217</v>
       </c>
-      <c r="B75" s="17">
+      <c r="B75" s="16">
         <v>29.9773999867258</v>
       </c>
       <c r="C75" s="1">
@@ -6022,7 +6334,7 @@
       <c r="T75" s="1">
         <v>192.929139543617</v>
       </c>
-      <c r="U75" s="18">
+      <c r="U75" s="17">
         <v>1.64913070426648</v>
       </c>
     </row>
@@ -6030,7 +6342,7 @@
       <c r="A76" s="8">
         <v>218</v>
       </c>
-      <c r="B76" s="17">
+      <c r="B76" s="16">
         <v>119.821509237049</v>
       </c>
       <c r="C76" s="1">
@@ -6087,7 +6399,7 @@
       <c r="T76" s="1">
         <v>100.80511818483301</v>
       </c>
-      <c r="U76" s="18">
+      <c r="U76" s="17">
         <v>80.255084642495007</v>
       </c>
     </row>
@@ -6095,7 +6407,7 @@
       <c r="A77" s="8">
         <v>219</v>
       </c>
-      <c r="B77" s="17">
+      <c r="B77" s="16">
         <v>170.36475152606101</v>
       </c>
       <c r="C77" s="1">
@@ -6152,7 +6464,7 @@
       <c r="T77" s="1">
         <v>214.07415487161799</v>
       </c>
-      <c r="U77" s="18">
+      <c r="U77" s="17">
         <v>7.5757897491478801</v>
       </c>
     </row>
@@ -6160,7 +6472,7 @@
       <c r="A78" s="8">
         <v>220</v>
       </c>
-      <c r="B78" s="17">
+      <c r="B78" s="16">
         <v>93.440763187399497</v>
       </c>
       <c r="C78" s="1">
@@ -6217,7 +6529,7 @@
       <c r="T78" s="1">
         <v>701.58491725843703</v>
       </c>
-      <c r="U78" s="18">
+      <c r="U78" s="17">
         <v>31.177473834540798</v>
       </c>
     </row>
@@ -6225,7 +6537,7 @@
       <c r="A79" s="8">
         <v>221</v>
       </c>
-      <c r="B79" s="17">
+      <c r="B79" s="16">
         <v>73.681464103585895</v>
       </c>
       <c r="C79" s="1">
@@ -6282,7 +6594,7 @@
       <c r="T79" s="1">
         <v>363.800834351091</v>
       </c>
-      <c r="U79" s="18">
+      <c r="U79" s="17">
         <v>24.3235267965769</v>
       </c>
     </row>
@@ -6290,7 +6602,7 @@
       <c r="A80" s="8">
         <v>222</v>
       </c>
-      <c r="B80" s="17">
+      <c r="B80" s="16">
         <v>79.657630047900298</v>
       </c>
       <c r="C80" s="1">
@@ -6347,7 +6659,7 @@
       <c r="T80" s="1">
         <v>0.59392001290748697</v>
       </c>
-      <c r="U80" s="18">
+      <c r="U80" s="17">
         <v>1.4178983074695899</v>
       </c>
     </row>
@@ -6355,7 +6667,7 @@
       <c r="A81" s="8">
         <v>223</v>
       </c>
-      <c r="B81" s="17">
+      <c r="B81" s="16">
         <v>55.223233586291997</v>
       </c>
       <c r="C81" s="1">
@@ -6412,7 +6724,7 @@
       <c r="T81" s="1">
         <v>667.00972379602695</v>
       </c>
-      <c r="U81" s="18">
+      <c r="U81" s="17">
         <v>29.902854177602801</v>
       </c>
     </row>
@@ -6420,7 +6732,7 @@
       <c r="A82" s="8">
         <v>224</v>
       </c>
-      <c r="B82" s="17">
+      <c r="B82" s="16">
         <v>19.111929176956899</v>
       </c>
       <c r="C82" s="1">
@@ -6477,7 +6789,7 @@
       <c r="T82" s="1">
         <v>4.6543940552071197</v>
       </c>
-      <c r="U82" s="18">
+      <c r="U82" s="17">
         <v>42.1497705544284</v>
       </c>
     </row>
@@ -6485,7 +6797,7 @@
       <c r="A83" s="8">
         <v>225</v>
       </c>
-      <c r="B83" s="17">
+      <c r="B83" s="16">
         <v>78.263635835328799</v>
       </c>
       <c r="C83" s="1">
@@ -6542,7 +6854,7 @@
       <c r="T83" s="1">
         <v>42.030828152008297</v>
       </c>
-      <c r="U83" s="18">
+      <c r="U83" s="17">
         <v>41.702931012847401</v>
       </c>
     </row>
@@ -6550,7 +6862,7 @@
       <c r="A84" s="8">
         <v>226</v>
       </c>
-      <c r="B84" s="17">
+      <c r="B84" s="16">
         <v>0.14212280511315101</v>
       </c>
       <c r="C84" s="1">
@@ -6607,7 +6919,7 @@
       <c r="T84" s="1">
         <v>34.829017570365401</v>
       </c>
-      <c r="U84" s="18">
+      <c r="U84" s="17">
         <v>108.35421491501501</v>
       </c>
     </row>
@@ -6615,7 +6927,7 @@
       <c r="A85" s="8">
         <v>227</v>
       </c>
-      <c r="B85" s="17">
+      <c r="B85" s="16">
         <v>150.34171444090799</v>
       </c>
       <c r="C85" s="1">
@@ -6672,7 +6984,7 @@
       <c r="T85" s="1">
         <v>1.6134527894719499</v>
       </c>
-      <c r="U85" s="18">
+      <c r="U85" s="17">
         <v>2.23831622473381</v>
       </c>
     </row>
@@ -6680,7 +6992,7 @@
       <c r="A86" s="8">
         <v>228</v>
       </c>
-      <c r="B86" s="17">
+      <c r="B86" s="16">
         <v>87.732857360266706</v>
       </c>
       <c r="C86" s="1">
@@ -6737,7 +7049,7 @@
       <c r="T86" s="1">
         <v>0.61974830364643196</v>
       </c>
-      <c r="U86" s="18">
+      <c r="U86" s="17">
         <v>281.89691861372597</v>
       </c>
     </row>
@@ -6745,7 +7057,7 @@
       <c r="A87" s="8">
         <v>229</v>
       </c>
-      <c r="B87" s="17">
+      <c r="B87" s="16">
         <v>67.963385965402196</v>
       </c>
       <c r="C87" s="1">
@@ -6802,7 +7114,7 @@
       <c r="T87" s="1">
         <v>135.72739614849201</v>
       </c>
-      <c r="U87" s="18">
+      <c r="U87" s="17">
         <v>69.322088508553193</v>
       </c>
     </row>
@@ -6810,7 +7122,7 @@
       <c r="A88" s="8">
         <v>230</v>
       </c>
-      <c r="B88" s="17">
+      <c r="B88" s="16">
         <v>18.415012003156399</v>
       </c>
       <c r="C88" s="1">
@@ -6867,7 +7179,7 @@
       <c r="T88" s="1">
         <v>709.12557826072805</v>
       </c>
-      <c r="U88" s="18">
+      <c r="U88" s="17">
         <v>49.101877732358503</v>
       </c>
     </row>
@@ -6875,7 +7187,7 @@
       <c r="A89" s="8">
         <v>231</v>
       </c>
-      <c r="B89" s="17">
+      <c r="B89" s="16">
         <v>24.272450629615001</v>
       </c>
       <c r="C89" s="1">
@@ -6932,7 +7244,7 @@
       <c r="T89" s="1">
         <v>491.408540170165</v>
       </c>
-      <c r="U89" s="18">
+      <c r="U89" s="17">
         <v>24.259053798274302</v>
       </c>
     </row>
@@ -6940,7 +7252,7 @@
       <c r="A90" s="8">
         <v>232</v>
       </c>
-      <c r="B90" s="17">
+      <c r="B90" s="16">
         <v>50.292785992011602</v>
       </c>
       <c r="C90" s="1">
@@ -6997,7 +7309,7 @@
       <c r="T90" s="1">
         <v>351.93895470380602</v>
       </c>
-      <c r="U90" s="18">
+      <c r="U90" s="17">
         <v>130.256952300959</v>
       </c>
     </row>
@@ -7005,7 +7317,7 @@
       <c r="A91" s="8">
         <v>233</v>
       </c>
-      <c r="B91" s="17">
+      <c r="B91" s="16">
         <v>91.2899255657737</v>
       </c>
       <c r="C91" s="1">
@@ -7062,7 +7374,7 @@
       <c r="T91" s="1">
         <v>304.91298708119598</v>
       </c>
-      <c r="U91" s="18">
+      <c r="U91" s="17">
         <v>1.1595699148341601</v>
       </c>
     </row>
@@ -7070,7 +7382,7 @@
       <c r="A92" s="8">
         <v>234</v>
       </c>
-      <c r="B92" s="17">
+      <c r="B92" s="16">
         <v>281.71669568869902</v>
       </c>
       <c r="C92" s="1">
@@ -7127,7 +7439,7 @@
       <c r="T92" s="1">
         <v>421.21239619289099</v>
       </c>
-      <c r="U92" s="18">
+      <c r="U92" s="17">
         <v>26.186667698036199</v>
       </c>
     </row>
@@ -7135,7 +7447,7 @@
       <c r="A93" s="8">
         <v>235</v>
       </c>
-      <c r="B93" s="17">
+      <c r="B93" s="16">
         <v>119.060523972398</v>
       </c>
       <c r="C93" s="1">
@@ -7192,7 +7504,7 @@
       <c r="T93" s="1">
         <v>616.43597767114602</v>
       </c>
-      <c r="U93" s="18">
+      <c r="U93" s="17">
         <v>22.746480296591901</v>
       </c>
     </row>
@@ -7200,7 +7512,7 @@
       <c r="A94" s="8">
         <v>236</v>
       </c>
-      <c r="B94" s="17">
+      <c r="B94" s="16">
         <v>46.580849615791202</v>
       </c>
       <c r="C94" s="1">
@@ -7257,7 +7569,7 @@
       <c r="T94" s="1">
         <v>5.5026856923514202</v>
       </c>
-      <c r="U94" s="18">
+      <c r="U94" s="17">
         <v>88.034071649511901</v>
       </c>
     </row>
@@ -7265,7 +7577,7 @@
       <c r="A95" s="8">
         <v>237</v>
       </c>
-      <c r="B95" s="17">
+      <c r="B95" s="16">
         <v>2.33338304715538</v>
       </c>
       <c r="C95" s="1">
@@ -7322,7 +7634,7 @@
       <c r="T95" s="1">
         <v>168.04788835444199</v>
       </c>
-      <c r="U95" s="18">
+      <c r="U95" s="17">
         <v>115.089864701694</v>
       </c>
     </row>
@@ -7330,7 +7642,7 @@
       <c r="A96" s="8">
         <v>238</v>
       </c>
-      <c r="B96" s="17">
+      <c r="B96" s="16">
         <v>57.447595228694396</v>
       </c>
       <c r="C96" s="1">
@@ -7387,15 +7699,15 @@
       <c r="T96" s="1">
         <v>91.722722564084705</v>
       </c>
-      <c r="U96" s="18">
+      <c r="U96" s="17">
         <v>366.20461894583599</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <v>239</v>
       </c>
-      <c r="B97" s="17">
+      <c r="B97" s="16">
         <v>68.948057665002594</v>
       </c>
       <c r="C97" s="1">
@@ -7452,15 +7764,15 @@
       <c r="T97" s="1">
         <v>240.78988693338701</v>
       </c>
-      <c r="U97" s="18">
+      <c r="U97" s="17">
         <v>942.46667622685595</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <v>240</v>
       </c>
-      <c r="B98" s="17">
+      <c r="B98" s="16">
         <v>24.316741162659302</v>
       </c>
       <c r="C98" s="1">
@@ -7517,15 +7829,15 @@
       <c r="T98" s="1">
         <v>324.70628124349201</v>
       </c>
-      <c r="U98" s="18">
+      <c r="U98" s="17">
         <v>363.31006732297698</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <v>241</v>
       </c>
-      <c r="B99" s="17">
+      <c r="B99" s="16">
         <v>188.18669611534099</v>
       </c>
       <c r="C99" s="1">
@@ -7582,15 +7894,15 @@
       <c r="T99" s="1">
         <v>532.76483298703499</v>
       </c>
-      <c r="U99" s="18">
+      <c r="U99" s="17">
         <v>1176.4931637027</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
         <v>242</v>
       </c>
-      <c r="B100" s="17">
+      <c r="B100" s="16">
         <v>27.5924213809961</v>
       </c>
       <c r="C100" s="1">
@@ -7647,15 +7959,15 @@
       <c r="T100" s="1">
         <v>994.79623194062901</v>
       </c>
-      <c r="U100" s="18">
+      <c r="U100" s="17">
         <v>456.69596005868101</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" s="8">
         <v>243</v>
       </c>
-      <c r="B101" s="17">
+      <c r="B101" s="16">
         <v>12.7889936337923</v>
       </c>
       <c r="C101" s="1">
@@ -7712,15 +8024,15 @@
       <c r="T101" s="1">
         <v>285.50418490691197</v>
       </c>
-      <c r="U101" s="18">
+      <c r="U101" s="17">
         <v>1249.36606584944</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" s="8">
         <v>244</v>
       </c>
-      <c r="B102" s="17">
+      <c r="B102" s="16">
         <v>108.197521592524</v>
       </c>
       <c r="C102" s="1">
@@ -7777,15 +8089,15 @@
       <c r="T102" s="1">
         <v>355.13078026417702</v>
       </c>
-      <c r="U102" s="18">
+      <c r="U102" s="17">
         <v>664.35335575985096</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <v>245</v>
       </c>
-      <c r="B103" s="17">
+      <c r="B103" s="16">
         <v>3.23553750804935</v>
       </c>
       <c r="C103" s="1">
@@ -7842,15 +8154,15 @@
       <c r="T103" s="1">
         <v>4.2505568145190296</v>
       </c>
-      <c r="U103" s="18">
+      <c r="U103" s="17">
         <v>654.30058124727896</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" s="8">
         <v>246</v>
       </c>
-      <c r="B104" s="17">
+      <c r="B104" s="16">
         <v>89.309115617501604</v>
       </c>
       <c r="C104" s="1">
@@ -7907,15 +8219,15 @@
       <c r="T104" s="1">
         <v>335.315644296892</v>
       </c>
-      <c r="U104" s="18">
+      <c r="U104" s="17">
         <v>400.57377526540103</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="9">
         <v>247</v>
       </c>
-      <c r="B105" s="20">
+      <c r="B105" s="19">
         <v>3.07916420882162</v>
       </c>
       <c r="C105" s="10">
@@ -7972,12 +8284,12 @@
       <c r="T105" s="10">
         <v>448.07857631114899</v>
       </c>
-      <c r="U105" s="21">
+      <c r="U105" s="20">
         <v>711.77358159756602</v>
       </c>
     </row>
-    <row r="106" spans="1:21" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="27" t="s">
+    <row r="106" spans="1:23" s="38" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B106" s="11">
@@ -8037,76 +8349,736 @@
       <c r="T106" s="12">
         <v>17805.790822712399</v>
       </c>
-      <c r="U106" s="22">
+      <c r="U106" s="21">
         <v>31061.5810070349</v>
       </c>
     </row>
-    <row r="107" spans="1:21" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="26" t="s">
+    <row r="107" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B107" s="23">
+      <c r="B107" s="39">
         <v>164.99749695003501</v>
       </c>
-      <c r="C107" s="13">
+      <c r="C107" s="40">
         <v>112.228027215559</v>
       </c>
-      <c r="D107" s="13">
+      <c r="D107" s="40">
         <v>80.5989667625457</v>
       </c>
-      <c r="E107" s="13">
+      <c r="E107" s="40">
         <v>400.68527566727101</v>
       </c>
-      <c r="F107" s="13">
+      <c r="F107" s="40">
         <v>55.234398369686502</v>
       </c>
-      <c r="G107" s="13">
+      <c r="G107" s="40">
         <v>198.63362964283101</v>
       </c>
-      <c r="H107" s="13">
+      <c r="H107" s="40">
         <v>123.299678772796</v>
       </c>
-      <c r="I107" s="13">
+      <c r="I107" s="40">
         <v>117.36799843211899</v>
       </c>
-      <c r="J107" s="13">
+      <c r="J107" s="40">
         <v>357.996136772189</v>
       </c>
-      <c r="K107" s="13">
+      <c r="K107" s="40">
         <v>127.979862218031</v>
       </c>
-      <c r="L107" s="13">
+      <c r="L107" s="40">
         <v>178.96813555334001</v>
       </c>
-      <c r="M107" s="13">
+      <c r="M107" s="40">
         <v>75.727682536596603</v>
       </c>
-      <c r="N107" s="13">
+      <c r="N107" s="40">
         <v>69.764207250338103</v>
       </c>
-      <c r="O107" s="13">
+      <c r="O107" s="40">
         <v>40.384816501307</v>
       </c>
-      <c r="P107" s="13">
+      <c r="P107" s="40">
         <v>40.384816501305998</v>
       </c>
-      <c r="Q107" s="13">
+      <c r="Q107" s="40">
         <v>308.42922264843003</v>
       </c>
-      <c r="R107" s="13">
+      <c r="R107" s="40">
         <v>103.87834323926501</v>
       </c>
-      <c r="S107" s="13">
+      <c r="S107" s="40">
         <v>270.377835037892</v>
       </c>
-      <c r="T107" s="13">
+      <c r="T107" s="40">
         <v>171.209527141466</v>
       </c>
-      <c r="U107" s="24">
+      <c r="U107" s="41">
         <v>298.66904814456598</v>
       </c>
     </row>
+    <row r="108" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="30">
+        <v>3</v>
+      </c>
+      <c r="B108" s="31">
+        <v>37358.745517000003</v>
+      </c>
+      <c r="C108" s="31">
+        <v>28148.977627699998</v>
+      </c>
+      <c r="D108" s="31">
+        <v>45057.311510799998</v>
+      </c>
+      <c r="E108" s="31">
+        <v>23755.507646099999</v>
+      </c>
+      <c r="F108" s="31">
+        <v>3762.4906298000001</v>
+      </c>
+      <c r="G108" s="31">
+        <v>28107.904547300001</v>
+      </c>
+      <c r="H108" s="31">
+        <v>12266.047646000001</v>
+      </c>
+      <c r="I108" s="31">
+        <v>3179280.01021</v>
+      </c>
+      <c r="J108" s="31">
+        <v>34955.912040800002</v>
+      </c>
+      <c r="K108" s="31">
+        <v>30527.8521048</v>
+      </c>
+      <c r="L108" s="31">
+        <v>26964.3784586</v>
+      </c>
+      <c r="M108" s="31">
+        <v>14109.9270089</v>
+      </c>
+      <c r="N108" s="31">
+        <v>7532859128</v>
+      </c>
+      <c r="O108" s="31">
+        <v>2440.8958397900001</v>
+      </c>
+      <c r="P108" s="31">
+        <v>38112.229176100001</v>
+      </c>
+      <c r="Q108" s="31">
+        <v>161879.476502</v>
+      </c>
+      <c r="R108" s="31">
+        <v>29408.958609900001</v>
+      </c>
+      <c r="S108" s="31">
+        <v>166662.00752799999</v>
+      </c>
+      <c r="T108" s="31">
+        <v>49933.076868999997</v>
+      </c>
+      <c r="U108" s="31">
+        <v>89483.030446899997</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="30"/>
+      <c r="B109" s="31">
+        <v>359.21870689399998</v>
+      </c>
+      <c r="C109" s="31">
+        <v>270.663246421</v>
+      </c>
+      <c r="D109" s="31">
+        <v>433.24337991099998</v>
+      </c>
+      <c r="E109" s="32">
+        <v>228.41834275100001</v>
+      </c>
+      <c r="F109" s="32">
+        <v>36.177794517300001</v>
+      </c>
+      <c r="G109" s="31">
+        <v>270.268312955</v>
+      </c>
+      <c r="H109" s="32">
+        <v>117.942765827</v>
+      </c>
+      <c r="I109" s="31">
+        <v>30570.000098199998</v>
+      </c>
+      <c r="J109" s="32">
+        <v>336.11453885399999</v>
+      </c>
+      <c r="K109" s="31">
+        <v>293.53703946899998</v>
+      </c>
+      <c r="L109" s="31">
+        <v>259.27286979399997</v>
+      </c>
+      <c r="M109" s="31">
+        <v>135.67237508599999</v>
+      </c>
+      <c r="N109" s="31">
+        <v>72431337.769199997</v>
+      </c>
+      <c r="O109" s="32">
+        <v>23.470152305700001</v>
+      </c>
+      <c r="P109" s="31">
+        <v>366.463742078</v>
+      </c>
+      <c r="Q109" s="31">
+        <v>1556.5334279000001</v>
+      </c>
+      <c r="R109" s="31">
+        <v>282.77844817300002</v>
+      </c>
+      <c r="S109" s="31">
+        <v>1602.5193031599999</v>
+      </c>
+      <c r="T109" s="31">
+        <v>480.125739125</v>
+      </c>
+      <c r="U109" s="31">
+        <v>860.41375429699997</v>
+      </c>
+      <c r="V109" s="26">
+        <f>SUM(B109:U109)</f>
+        <v>72469820.603237718</v>
+      </c>
+      <c r="W109" s="26">
+        <f>V109/20</f>
+        <v>3623491.030161886</v>
+      </c>
+    </row>
+    <row r="110" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="48">
+        <v>4</v>
+      </c>
+      <c r="B110" s="49">
+        <v>27460.4418931</v>
+      </c>
+      <c r="C110" s="49">
+        <v>19370.307719699998</v>
+      </c>
+      <c r="D110" s="49">
+        <v>14219.011034900001</v>
+      </c>
+      <c r="E110" s="49">
+        <v>24698.834751499999</v>
+      </c>
+      <c r="F110" s="49">
+        <v>6811.3987406400001</v>
+      </c>
+      <c r="G110" s="49">
+        <v>39549.776564899999</v>
+      </c>
+      <c r="H110" s="49">
+        <v>12715.3132042</v>
+      </c>
+      <c r="I110" s="49">
+        <v>34995.379671399998</v>
+      </c>
+      <c r="J110" s="49">
+        <v>39289.896746099999</v>
+      </c>
+      <c r="K110" s="49">
+        <v>21265.686675500001</v>
+      </c>
+      <c r="L110" s="49">
+        <v>34756.449921699998</v>
+      </c>
+      <c r="M110" s="49">
+        <v>14157.8313361</v>
+      </c>
+      <c r="N110" s="49">
+        <v>23834.417611100002</v>
+      </c>
+      <c r="O110" s="49">
+        <v>2267.8282804700002</v>
+      </c>
+      <c r="P110" s="49">
+        <v>3596.8106818199999</v>
+      </c>
+      <c r="Q110" s="49">
+        <v>69625.387884399999</v>
+      </c>
+      <c r="R110" s="49">
+        <v>26464.8856705</v>
+      </c>
+      <c r="S110" s="49">
+        <v>12180.917567300001</v>
+      </c>
+      <c r="T110" s="49">
+        <v>22952.030774499999</v>
+      </c>
+      <c r="U110" s="49">
+        <v>118309.648812</v>
+      </c>
+      <c r="V110" s="50"/>
+    </row>
+    <row r="111" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="48"/>
+      <c r="B111" s="49">
+        <v>264.042710511</v>
+      </c>
+      <c r="C111" s="49">
+        <v>186.25295884400001</v>
+      </c>
+      <c r="D111" s="49">
+        <v>136.72125995100001</v>
+      </c>
+      <c r="E111" s="49">
+        <v>237.48879568699999</v>
+      </c>
+      <c r="F111" s="49">
+        <v>65.494218660000001</v>
+      </c>
+      <c r="G111" s="49">
+        <v>380.286313124</v>
+      </c>
+      <c r="H111" s="51">
+        <v>122.262626963</v>
+      </c>
+      <c r="I111" s="49">
+        <v>336.49403530199999</v>
+      </c>
+      <c r="J111" s="49">
+        <v>377.78746871300001</v>
+      </c>
+      <c r="K111" s="49">
+        <v>204.47775649499999</v>
+      </c>
+      <c r="L111" s="49">
+        <v>334.19663386299999</v>
+      </c>
+      <c r="M111" s="49">
+        <v>136.13299361700001</v>
+      </c>
+      <c r="N111" s="49">
+        <v>229.17709241399999</v>
+      </c>
+      <c r="O111" s="51">
+        <v>21.806041158300001</v>
+      </c>
+      <c r="P111" s="51">
+        <v>34.584718094400003</v>
+      </c>
+      <c r="Q111" s="49">
+        <v>669.47488350399999</v>
+      </c>
+      <c r="R111" s="49">
+        <v>254.47005452400001</v>
+      </c>
+      <c r="S111" s="51">
+        <v>117.12420737799999</v>
+      </c>
+      <c r="T111" s="49">
+        <v>220.692603601</v>
+      </c>
+      <c r="U111" s="49">
+        <v>1137.5927770400001</v>
+      </c>
+      <c r="V111" s="50">
+        <f t="shared" ref="V110:V115" si="0">SUM(B111:U111)</f>
+        <v>5466.5601494437005</v>
+      </c>
+      <c r="W111" s="27">
+        <f>V111/20</f>
+        <v>273.32800747218505</v>
+      </c>
+    </row>
+    <row r="112" spans="1:23" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="33">
+        <v>5</v>
+      </c>
+      <c r="B112" s="34">
+        <v>19455.528460900001</v>
+      </c>
+      <c r="C112" s="34">
+        <v>36831.366647199997</v>
+      </c>
+      <c r="D112" s="34">
+        <v>16619.481868300001</v>
+      </c>
+      <c r="E112" s="34">
+        <v>31816.254222399999</v>
+      </c>
+      <c r="F112" s="34">
+        <v>3408.8993179600002</v>
+      </c>
+      <c r="G112" s="34">
+        <v>29848.338228199998</v>
+      </c>
+      <c r="H112" s="34">
+        <v>14570.7416512</v>
+      </c>
+      <c r="I112" s="34">
+        <v>46974.141749399998</v>
+      </c>
+      <c r="J112" s="34">
+        <v>47855.750460099996</v>
+      </c>
+      <c r="K112" s="34">
+        <v>35328.118900300004</v>
+      </c>
+      <c r="L112" s="34">
+        <v>17651.048396599999</v>
+      </c>
+      <c r="M112" s="34">
+        <v>15563.788933600001</v>
+      </c>
+      <c r="N112" s="34">
+        <v>22038.882111200001</v>
+      </c>
+      <c r="O112" s="34">
+        <v>1670.33962572</v>
+      </c>
+      <c r="P112" s="34">
+        <v>5799.1805206700001</v>
+      </c>
+      <c r="Q112" s="34">
+        <v>19756.070047900001</v>
+      </c>
+      <c r="R112" s="34">
+        <v>17790.9325245</v>
+      </c>
+      <c r="S112" s="34">
+        <v>16087.749815900001</v>
+      </c>
+      <c r="T112" s="34">
+        <v>19574.1229958</v>
+      </c>
+      <c r="U112" s="34">
+        <v>78841.273471099994</v>
+      </c>
+      <c r="V112" s="45"/>
+    </row>
+    <row r="113" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="33"/>
+      <c r="B113" s="34">
+        <v>187.072389047</v>
+      </c>
+      <c r="C113" s="34">
+        <v>354.14775622299999</v>
+      </c>
+      <c r="D113" s="34">
+        <v>159.80271027200001</v>
+      </c>
+      <c r="E113" s="34">
+        <v>305.92552136900002</v>
+      </c>
+      <c r="F113" s="35">
+        <v>32.777878057300001</v>
+      </c>
+      <c r="G113" s="34">
+        <v>287.00325219400003</v>
+      </c>
+      <c r="H113" s="34">
+        <v>140.10328510799999</v>
+      </c>
+      <c r="I113" s="34">
+        <v>451.674439898</v>
+      </c>
+      <c r="J113" s="34">
+        <v>460.15144673200001</v>
+      </c>
+      <c r="K113" s="34">
+        <v>339.69345096400002</v>
+      </c>
+      <c r="L113" s="35">
+        <v>169.72161919800001</v>
+      </c>
+      <c r="M113" s="34">
+        <v>149.651816669</v>
+      </c>
+      <c r="N113" s="34">
+        <v>211.912327992</v>
+      </c>
+      <c r="O113" s="35">
+        <v>16.060957939600002</v>
+      </c>
+      <c r="P113" s="34">
+        <v>55.761351160300002</v>
+      </c>
+      <c r="Q113" s="35">
+        <v>189.962211999</v>
+      </c>
+      <c r="R113" s="34">
+        <v>171.066658889</v>
+      </c>
+      <c r="S113" s="35">
+        <v>154.68990207600001</v>
+      </c>
+      <c r="T113" s="34">
+        <v>188.21272111299999</v>
+      </c>
+      <c r="U113" s="34">
+        <v>758.08916799099995</v>
+      </c>
+      <c r="V113" s="45">
+        <f t="shared" si="0"/>
+        <v>4783.4808648911994</v>
+      </c>
+      <c r="W113" s="25">
+        <f>V113/20</f>
+        <v>239.17404324455998</v>
+      </c>
+    </row>
+    <row r="114" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="36">
+        <v>6</v>
+      </c>
+      <c r="B114" s="37">
+        <v>26921.8215098</v>
+      </c>
+      <c r="C114" s="37">
+        <v>28677.640186299999</v>
+      </c>
+      <c r="D114" s="37">
+        <v>24861.734785199998</v>
+      </c>
+      <c r="E114" s="37">
+        <v>110776.71392900001</v>
+      </c>
+      <c r="F114" s="37">
+        <v>2993.75698371</v>
+      </c>
+      <c r="G114" s="37">
+        <v>29940.7345661</v>
+      </c>
+      <c r="H114" s="37">
+        <v>8256.1330484600003</v>
+      </c>
+      <c r="I114" s="37">
+        <v>42134.900773900001</v>
+      </c>
+      <c r="J114" s="37">
+        <v>41146.3352199</v>
+      </c>
+      <c r="K114" s="37">
+        <v>35497.699881400004</v>
+      </c>
+      <c r="L114" s="37">
+        <v>25982.719393399999</v>
+      </c>
+      <c r="M114" s="37">
+        <v>8758.6512665200007</v>
+      </c>
+      <c r="N114" s="37">
+        <v>15294.252718</v>
+      </c>
+      <c r="O114" s="37">
+        <v>115899.42303599999</v>
+      </c>
+      <c r="P114" s="37">
+        <v>2591.3519432100002</v>
+      </c>
+      <c r="Q114" s="37">
+        <v>35497.114962899999</v>
+      </c>
+      <c r="R114" s="37">
+        <v>11810.5707791</v>
+      </c>
+      <c r="S114" s="37">
+        <v>33886.1813502</v>
+      </c>
+      <c r="T114" s="37">
+        <v>23039.208666800001</v>
+      </c>
+      <c r="U114" s="37">
+        <v>348347.20829699998</v>
+      </c>
+      <c r="V114" s="47"/>
+    </row>
+    <row r="115" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="36"/>
+      <c r="B115" s="52">
+        <v>258.86366836299999</v>
+      </c>
+      <c r="C115" s="52">
+        <v>275.74654025299998</v>
+      </c>
+      <c r="D115" s="52">
+        <v>239.05514216500001</v>
+      </c>
+      <c r="E115" s="52">
+        <v>1065.16071085</v>
+      </c>
+      <c r="F115" s="53">
+        <v>28.786124843300001</v>
+      </c>
+      <c r="G115" s="52">
+        <v>287.89167852100002</v>
+      </c>
+      <c r="H115" s="53">
+        <v>79.385894696700007</v>
+      </c>
+      <c r="I115" s="52">
+        <v>405.14327667200001</v>
+      </c>
+      <c r="J115" s="52">
+        <v>395.63783865300002</v>
+      </c>
+      <c r="K115" s="52">
+        <v>341.32403732099999</v>
+      </c>
+      <c r="L115" s="52">
+        <v>249.833840321</v>
+      </c>
+      <c r="M115" s="52">
+        <v>84.2178006396</v>
+      </c>
+      <c r="N115" s="52">
+        <v>147.06012228899999</v>
+      </c>
+      <c r="O115" s="52">
+        <v>1114.4175292</v>
+      </c>
+      <c r="P115" s="53">
+        <v>24.916845607799999</v>
+      </c>
+      <c r="Q115" s="52">
+        <v>341.318413104</v>
+      </c>
+      <c r="R115" s="52">
+        <v>113.56318056800001</v>
+      </c>
+      <c r="S115" s="52">
+        <v>325.82866682899999</v>
+      </c>
+      <c r="T115" s="52">
+        <v>221.53085256599999</v>
+      </c>
+      <c r="U115" s="52">
+        <v>3349.4923874699998</v>
+      </c>
+      <c r="V115" s="47">
+        <f t="shared" si="0"/>
+        <v>9349.1745509323991</v>
+      </c>
+      <c r="W115" s="28">
+        <f>V115/20</f>
+        <v>467.45872754661997</v>
+      </c>
+    </row>
+    <row r="116" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="43">
+        <v>7</v>
+      </c>
+      <c r="B116" s="44">
+        <v>20274.647340799998</v>
+      </c>
+    </row>
+    <row r="117" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="43"/>
+      <c r="B117" s="44">
+        <v>194.94853212300001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:23" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="54">
+        <v>8</v>
+      </c>
+      <c r="B118" s="55">
+        <v>23855.423083400001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:23" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="54"/>
+      <c r="B119" s="55">
+        <v>229.37906810999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:23" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="57">
+        <v>9</v>
+      </c>
+      <c r="B120" s="58">
+        <v>21923.905306600001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:23" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="57"/>
+      <c r="B121" s="58">
+        <v>210.80678179500001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:23" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="60">
+        <v>10</v>
+      </c>
+      <c r="B122" s="46">
+        <v>25974.9545082</v>
+      </c>
+    </row>
+    <row r="123" spans="1:23" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="61"/>
+      <c r="B123" s="46">
+        <v>249.75917796300001</v>
+      </c>
+    </row>
+    <row r="124" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="62">
+        <v>10</v>
+      </c>
+      <c r="B124" s="59">
+        <v>48199.039138200002</v>
+      </c>
+    </row>
+    <row r="125" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="63"/>
+      <c r="B125" s="59">
+        <v>463.45229940500002</v>
+      </c>
+    </row>
+    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A126" s="42">
+        <v>11</v>
+      </c>
+      <c r="B126">
+        <v>23117.037772</v>
+      </c>
+    </row>
+    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A127" s="56"/>
+      <c r="B127">
+        <v>222.27920934599999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A128" s="23">
+        <v>12</v>
+      </c>
+      <c r="B128">
+        <v>22660.990475899998</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="23"/>
+      <c r="B129">
+        <v>217.89413919099999</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="A110:A111"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A119"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Resultados de pruebas :/"
This reverts commit 3ac37129949a9f6d3e8d2a9bbfeb5491e82a7502.
</commit_message>
<xml_diff>
--- a/Results - Gustavo - 1010101010.xlsx
+++ b/Results - Gustavo - 1010101010.xlsx
@@ -4,172 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="RRR" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>vanecan</author>
-  </authors>
-  <commentList>
-    <comment ref="A112" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>num_generations = 10000
-population_size = 500
-pool_size = 4
-const_max = 10.0
-step_size_const = 2
-p_reg_op2_const = 0.7
-p_const_in = 0.7
-p_macro_mutation = 0.45
-p_ins = 0.7
-p_del = 0.3
-p_micro_mutation = 0.95
-p_regmut = 0.5 
-p_opermut = 0.40
-p_constmut = 0.1
-p_crossover = 0.05</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A120" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>num_generations = 10000
-population_size = 500
-const_max = 25.0
-step_size_const = 2 
-p_reg_op2_const = 0.7
-p_const_in = 0.8
-p_macro_mutation = 0.6
-p_ins = 0.7 
-p_del = 0.3
-p_micro_mutation = 0.95
-p_regmut = 0.5 
-p_opermut = 0.40 
-p_constmut = 0.1 
-p_crossover = 0.05</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A122" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> num_generations = 10000
- population_size = 500
- pool_size = 4
- const_max = 10.0
- step_size_const = 0.5
- p_reg_op2_const = 0.7
- p_const_in = 0.7
- p_macro_mutation = 0.4
- p_ins = 0.7
- p_del = 0.3
- p_micro_mutation = 0.95
- p_regmut = 0.5
- p_opermut = 0.40
- p_constmut = 0.1 
- p_crossover = 0.2</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A124" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>num_generations = 10000
-population_size = 500
-pool_size = 4
-const_max = 5.0
-step_size_const = 2 
-p_reg_op2_const = 0.7
-p_const_in = 0.8
-p_macro_mutation = 0.6
-p_ins = 0.7
-p_del = 0.3
-p_micro_mutation = 0.95
-p_regmut = 0.5
-p_opermut = 0.40
-p_constmut = 0.1 
-p_crossover = 0.05</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A126" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>num_generations = 10000
-population_size = 500
-pool_size = 4
-const_max = 10.0
-step_size_const = 0.5
-p_reg_op2_const = 0.7
-p_const_in = 0.7
-p_macro_mutation = 0.4
-p_ins = 0.7
-p_del = 0.3
-p_micro_mutation = 0.95
-p_regmut = 0.5
-p_opermut = 0.40
-p_constmut = 0.1 
-p_crossover = 0.05</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -185,7 +26,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,21 +162,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="43">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -523,6 +351,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -535,48 +369,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -837,6 +635,19 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -915,65 +726,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1019,99 +771,35 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="41" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1453,11 +1141,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W129"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A107" sqref="A1:XFD107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,7 +1155,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="13">
+      <c r="B1" s="14">
         <v>1</v>
       </c>
       <c r="C1" s="4">
@@ -1532,7 +1220,7 @@
       <c r="A2" s="7">
         <v>144</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="15">
         <v>21.468403494018901</v>
       </c>
       <c r="C2" s="3">
@@ -1589,7 +1277,7 @@
       <c r="T2" s="3">
         <v>122.974149078835</v>
       </c>
-      <c r="U2" s="15">
+      <c r="U2" s="16">
         <v>18.832553116792202</v>
       </c>
     </row>
@@ -1597,7 +1285,7 @@
       <c r="A3" s="8">
         <v>145</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="17">
         <v>30.621474445603099</v>
       </c>
       <c r="C3" s="1">
@@ -1654,7 +1342,7 @@
       <c r="T3" s="1">
         <v>52.823391488371698</v>
       </c>
-      <c r="U3" s="17">
+      <c r="U3" s="18">
         <v>66.801683974615798</v>
       </c>
     </row>
@@ -1662,7 +1350,7 @@
       <c r="A4" s="8">
         <v>146</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="17">
         <v>1.5929773377246701</v>
       </c>
       <c r="C4" s="1">
@@ -1719,7 +1407,7 @@
       <c r="T4" s="1">
         <v>256.26530248787202</v>
       </c>
-      <c r="U4" s="17">
+      <c r="U4" s="18">
         <v>0.412204063045151</v>
       </c>
     </row>
@@ -1727,7 +1415,7 @@
       <c r="A5" s="8">
         <v>147</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="17">
         <v>11.9480417717726</v>
       </c>
       <c r="C5" s="1">
@@ -1784,7 +1472,7 @@
       <c r="T5" s="1">
         <v>15.3769698195636</v>
       </c>
-      <c r="U5" s="17">
+      <c r="U5" s="18">
         <v>0.14802647062111901</v>
       </c>
     </row>
@@ -1792,7 +1480,7 @@
       <c r="A6" s="8">
         <v>148</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="17">
         <v>106.882758808185</v>
       </c>
       <c r="C6" s="1">
@@ -1849,7 +1537,7 @@
       <c r="T6" s="1">
         <v>46.142908673837397</v>
       </c>
-      <c r="U6" s="17">
+      <c r="U6" s="18">
         <v>4.2825350969779201</v>
       </c>
     </row>
@@ -1857,7 +1545,7 @@
       <c r="A7" s="8">
         <v>149</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="17">
         <v>15.5810151059757</v>
       </c>
       <c r="C7" s="1">
@@ -1914,7 +1602,7 @@
       <c r="T7" s="1">
         <v>138.926698206184</v>
       </c>
-      <c r="U7" s="17">
+      <c r="U7" s="18">
         <v>207.370382741116</v>
       </c>
     </row>
@@ -1922,7 +1610,7 @@
       <c r="A8" s="8">
         <v>150</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="17">
         <v>37.386624069382002</v>
       </c>
       <c r="C8" s="1">
@@ -1979,7 +1667,7 @@
       <c r="T8" s="1">
         <v>2.3206119491300901</v>
       </c>
-      <c r="U8" s="17">
+      <c r="U8" s="18">
         <v>82.134655714920797</v>
       </c>
     </row>
@@ -1987,7 +1675,7 @@
       <c r="A9" s="8">
         <v>151</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="17">
         <v>29.135478942174601</v>
       </c>
       <c r="C9" s="1">
@@ -2044,7 +1732,7 @@
       <c r="T9" s="1">
         <v>15.8860384616444</v>
       </c>
-      <c r="U9" s="17">
+      <c r="U9" s="18">
         <v>8.9899446694007192</v>
       </c>
     </row>
@@ -2052,7 +1740,7 @@
       <c r="A10" s="8">
         <v>152</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="17">
         <v>7.2095363708380598E-3</v>
       </c>
       <c r="C10" s="1">
@@ -2109,7 +1797,7 @@
       <c r="T10" s="1">
         <v>1.28521546362743</v>
       </c>
-      <c r="U10" s="17">
+      <c r="U10" s="18">
         <v>5.2497741289216604</v>
       </c>
     </row>
@@ -2117,7 +1805,7 @@
       <c r="A11" s="8">
         <v>153</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="17">
         <v>19.849076373651201</v>
       </c>
       <c r="C11" s="1">
@@ -2174,7 +1862,7 @@
       <c r="T11" s="1">
         <v>22.188168684704898</v>
       </c>
-      <c r="U11" s="17">
+      <c r="U11" s="18">
         <v>1.94586550165712</v>
       </c>
     </row>
@@ -2182,7 +1870,7 @@
       <c r="A12" s="8">
         <v>154</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="17">
         <v>1.85706346049278</v>
       </c>
       <c r="C12" s="1">
@@ -2239,7 +1927,7 @@
       <c r="T12" s="1">
         <v>38.807940921105804</v>
       </c>
-      <c r="U12" s="17">
+      <c r="U12" s="18">
         <v>0.44229397942567</v>
       </c>
     </row>
@@ -2247,7 +1935,7 @@
       <c r="A13" s="8">
         <v>155</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="17">
         <v>5.0563305451335196</v>
       </c>
       <c r="C13" s="1">
@@ -2304,7 +1992,7 @@
       <c r="T13" s="1">
         <v>0.98647139664379402</v>
       </c>
-      <c r="U13" s="17">
+      <c r="U13" s="18">
         <v>15.4046837816067</v>
       </c>
     </row>
@@ -2312,7 +2000,7 @@
       <c r="A14" s="8">
         <v>156</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="17">
         <v>2.7632499087792199</v>
       </c>
       <c r="C14" s="1">
@@ -2369,7 +2057,7 @@
       <c r="T14" s="1">
         <v>68.102185567857902</v>
       </c>
-      <c r="U14" s="17">
+      <c r="U14" s="18">
         <v>8.9533046928742301</v>
       </c>
     </row>
@@ -2377,7 +2065,7 @@
       <c r="A15" s="8">
         <v>157</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="17">
         <v>27.747334148459199</v>
       </c>
       <c r="C15" s="1">
@@ -2434,7 +2122,7 @@
       <c r="T15" s="1">
         <v>1.55767506298028</v>
       </c>
-      <c r="U15" s="17">
+      <c r="U15" s="18">
         <v>60.366556116807203</v>
       </c>
     </row>
@@ -2442,7 +2130,7 @@
       <c r="A16" s="8">
         <v>158</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="17">
         <v>254.16786565579599</v>
       </c>
       <c r="C16" s="1">
@@ -2499,7 +2187,7 @@
       <c r="T16" s="1">
         <v>9.9518333060017294</v>
       </c>
-      <c r="U16" s="17">
+      <c r="U16" s="18">
         <v>1.4154755195534401</v>
       </c>
     </row>
@@ -2507,7 +2195,7 @@
       <c r="A17" s="8">
         <v>159</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="17">
         <v>137.15898473867099</v>
       </c>
       <c r="C17" s="1">
@@ -2564,7 +2252,7 @@
       <c r="T17" s="1">
         <v>0.84890704532888495</v>
       </c>
-      <c r="U17" s="17">
+      <c r="U17" s="18">
         <v>8.3762370728515407E-3</v>
       </c>
     </row>
@@ -2572,7 +2260,7 @@
       <c r="A18" s="8">
         <v>160</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="17">
         <v>47.566716209700203</v>
       </c>
       <c r="C18" s="1">
@@ -2629,7 +2317,7 @@
       <c r="T18" s="1">
         <v>217.32540233068099</v>
       </c>
-      <c r="U18" s="17">
+      <c r="U18" s="18">
         <v>23.445475770823101</v>
       </c>
     </row>
@@ -2637,7 +2325,7 @@
       <c r="A19" s="8">
         <v>161</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="17">
         <v>313.49625264576099</v>
       </c>
       <c r="C19" s="1">
@@ -2694,7 +2382,7 @@
       <c r="T19" s="1">
         <v>4.5795257789600896</v>
       </c>
-      <c r="U19" s="17">
+      <c r="U19" s="18">
         <v>16.2067224727862</v>
       </c>
     </row>
@@ -2702,7 +2390,7 @@
       <c r="A20" s="8">
         <v>162</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="17">
         <v>145.70728520075099</v>
       </c>
       <c r="C20" s="1">
@@ -2759,7 +2447,7 @@
       <c r="T20" s="1">
         <v>170.10642944965801</v>
       </c>
-      <c r="U20" s="17">
+      <c r="U20" s="18">
         <v>170.39420035504801</v>
       </c>
     </row>
@@ -2767,7 +2455,7 @@
       <c r="A21" s="8">
         <v>163</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="17">
         <v>41.384606431698998</v>
       </c>
       <c r="C21" s="2">
@@ -2824,7 +2512,7 @@
       <c r="T21" s="1">
         <v>758.62577903299098</v>
       </c>
-      <c r="U21" s="17">
+      <c r="U21" s="18">
         <v>5.6554113715091301</v>
       </c>
     </row>
@@ -2832,7 +2520,7 @@
       <c r="A22" s="8">
         <v>164</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="17">
         <v>581.97887697430201</v>
       </c>
       <c r="C22" s="1">
@@ -2889,7 +2577,7 @@
       <c r="T22" s="1">
         <v>42.214175190134398</v>
       </c>
-      <c r="U22" s="18">
+      <c r="U22" s="19">
         <v>1.2016802140640201E-5</v>
       </c>
     </row>
@@ -2897,7 +2585,7 @@
       <c r="A23" s="8">
         <v>165</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23" s="17">
         <v>117.489151794066</v>
       </c>
       <c r="C23" s="1">
@@ -2954,7 +2642,7 @@
       <c r="T23" s="1">
         <v>155.23383950477299</v>
       </c>
-      <c r="U23" s="17">
+      <c r="U23" s="18">
         <v>44.509751461826298</v>
       </c>
     </row>
@@ -2962,7 +2650,7 @@
       <c r="A24" s="8">
         <v>166</v>
       </c>
-      <c r="B24" s="16">
+      <c r="B24" s="17">
         <v>88.531521544392902</v>
       </c>
       <c r="C24" s="1">
@@ -3019,7 +2707,7 @@
       <c r="T24" s="1">
         <v>40.148737497934</v>
       </c>
-      <c r="U24" s="17">
+      <c r="U24" s="18">
         <v>112.56814649866</v>
       </c>
     </row>
@@ -3027,7 +2715,7 @@
       <c r="A25" s="8">
         <v>167</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="17">
         <v>10.063841855633701</v>
       </c>
       <c r="C25" s="1">
@@ -3084,7 +2772,7 @@
       <c r="T25" s="1">
         <v>16.643191848894599</v>
       </c>
-      <c r="U25" s="17">
+      <c r="U25" s="18">
         <v>145.51150690750799</v>
       </c>
     </row>
@@ -3092,7 +2780,7 @@
       <c r="A26" s="8">
         <v>168</v>
       </c>
-      <c r="B26" s="16">
+      <c r="B26" s="17">
         <v>16.669373770350301</v>
       </c>
       <c r="C26" s="1">
@@ -3149,7 +2837,7 @@
       <c r="T26" s="1">
         <v>57.998591627398099</v>
       </c>
-      <c r="U26" s="17">
+      <c r="U26" s="18">
         <v>42.748456282381397</v>
       </c>
     </row>
@@ -3157,7 +2845,7 @@
       <c r="A27" s="8">
         <v>169</v>
       </c>
-      <c r="B27" s="16">
+      <c r="B27" s="17">
         <v>35.933421702320501</v>
       </c>
       <c r="C27" s="1">
@@ -3214,7 +2902,7 @@
       <c r="T27" s="1">
         <v>0.151932091547475</v>
       </c>
-      <c r="U27" s="17">
+      <c r="U27" s="18">
         <v>2.3899826409584901</v>
       </c>
     </row>
@@ -3222,7 +2910,7 @@
       <c r="A28" s="8">
         <v>170</v>
       </c>
-      <c r="B28" s="16">
+      <c r="B28" s="17">
         <v>84.200874843417694</v>
       </c>
       <c r="C28" s="1">
@@ -3279,7 +2967,7 @@
       <c r="T28" s="1">
         <v>241.394670162344</v>
       </c>
-      <c r="U28" s="17">
+      <c r="U28" s="18">
         <v>6.8815514754952803E-2</v>
       </c>
     </row>
@@ -3287,7 +2975,7 @@
       <c r="A29" s="8">
         <v>171</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B29" s="17">
         <v>237.80070089344201</v>
       </c>
       <c r="C29" s="1">
@@ -3344,7 +3032,7 @@
       <c r="T29" s="1">
         <v>219.76958913016199</v>
       </c>
-      <c r="U29" s="17">
+      <c r="U29" s="18">
         <v>37.340095628323198</v>
       </c>
     </row>
@@ -3352,7 +3040,7 @@
       <c r="A30" s="8">
         <v>172</v>
       </c>
-      <c r="B30" s="16">
+      <c r="B30" s="17">
         <v>379.48605407182998</v>
       </c>
       <c r="C30" s="1">
@@ -3409,7 +3097,7 @@
       <c r="T30" s="1">
         <v>586.63887522236905</v>
       </c>
-      <c r="U30" s="17">
+      <c r="U30" s="18">
         <v>33.027146264657397</v>
       </c>
     </row>
@@ -3417,7 +3105,7 @@
       <c r="A31" s="8">
         <v>173</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="17">
         <v>60.232342852935801</v>
       </c>
       <c r="C31" s="1">
@@ -3474,7 +3162,7 @@
       <c r="T31" s="1">
         <v>185.44950494372301</v>
       </c>
-      <c r="U31" s="17">
+      <c r="U31" s="18">
         <v>925.21845589971201</v>
       </c>
     </row>
@@ -3482,7 +3170,7 @@
       <c r="A32" s="8">
         <v>174</v>
       </c>
-      <c r="B32" s="16">
+      <c r="B32" s="17">
         <v>111.05763228253799</v>
       </c>
       <c r="C32" s="1">
@@ -3539,7 +3227,7 @@
       <c r="T32" s="1">
         <v>1056.5955160937999</v>
       </c>
-      <c r="U32" s="17">
+      <c r="U32" s="18">
         <v>330.08077997817003</v>
       </c>
     </row>
@@ -3547,7 +3235,7 @@
       <c r="A33" s="8">
         <v>175</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B33" s="17">
         <v>225.49497975204099</v>
       </c>
       <c r="C33" s="1">
@@ -3604,7 +3292,7 @@
       <c r="T33" s="1">
         <v>90.459727507147306</v>
       </c>
-      <c r="U33" s="17">
+      <c r="U33" s="18">
         <v>150.00506632117899</v>
       </c>
     </row>
@@ -3612,7 +3300,7 @@
       <c r="A34" s="8">
         <v>176</v>
       </c>
-      <c r="B34" s="16">
+      <c r="B34" s="17">
         <v>409.427888562367</v>
       </c>
       <c r="C34" s="1">
@@ -3669,7 +3357,7 @@
       <c r="T34" s="1">
         <v>58.2003220511519</v>
       </c>
-      <c r="U34" s="17">
+      <c r="U34" s="18">
         <v>22.602483075808198</v>
       </c>
     </row>
@@ -3677,7 +3365,7 @@
       <c r="A35" s="8">
         <v>177</v>
       </c>
-      <c r="B35" s="16">
+      <c r="B35" s="17">
         <v>164.14442234982999</v>
       </c>
       <c r="C35" s="1">
@@ -3734,7 +3422,7 @@
       <c r="T35" s="1">
         <v>46.872934496324902</v>
       </c>
-      <c r="U35" s="17">
+      <c r="U35" s="18">
         <v>299.13416121133702</v>
       </c>
     </row>
@@ -3742,7 +3430,7 @@
       <c r="A36" s="8">
         <v>178</v>
       </c>
-      <c r="B36" s="16">
+      <c r="B36" s="17">
         <v>53.869356435240803</v>
       </c>
       <c r="C36" s="1">
@@ -3799,7 +3487,7 @@
       <c r="T36" s="1">
         <v>356.70683461573998</v>
       </c>
-      <c r="U36" s="17">
+      <c r="U36" s="18">
         <v>284.84616150795603</v>
       </c>
     </row>
@@ -3807,7 +3495,7 @@
       <c r="A37" s="8">
         <v>179</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B37" s="17">
         <v>34.650742342693597</v>
       </c>
       <c r="C37" s="1">
@@ -3864,7 +3552,7 @@
       <c r="T37" s="1">
         <v>657.81074119787002</v>
       </c>
-      <c r="U37" s="17">
+      <c r="U37" s="18">
         <v>270.06709990417602</v>
       </c>
     </row>
@@ -3872,7 +3560,7 @@
       <c r="A38" s="8">
         <v>180</v>
       </c>
-      <c r="B38" s="16">
+      <c r="B38" s="17">
         <v>146.61351139565801</v>
       </c>
       <c r="C38" s="1">
@@ -3929,7 +3617,7 @@
       <c r="T38" s="1">
         <v>378.32526593877498</v>
       </c>
-      <c r="U38" s="17">
+      <c r="U38" s="18">
         <v>273.36342616621903</v>
       </c>
     </row>
@@ -3937,7 +3625,7 @@
       <c r="A39" s="8">
         <v>181</v>
       </c>
-      <c r="B39" s="16">
+      <c r="B39" s="17">
         <v>111.25458000453899</v>
       </c>
       <c r="C39" s="1">
@@ -3994,7 +3682,7 @@
       <c r="T39" s="1">
         <v>7.6907779583400799</v>
       </c>
-      <c r="U39" s="17">
+      <c r="U39" s="18">
         <v>452.09946477438098</v>
       </c>
     </row>
@@ -4002,7 +3690,7 @@
       <c r="A40" s="8">
         <v>182</v>
       </c>
-      <c r="B40" s="16">
+      <c r="B40" s="17">
         <v>120.807825308817</v>
       </c>
       <c r="C40" s="1">
@@ -4059,7 +3747,7 @@
       <c r="T40" s="1">
         <v>201.882022175879</v>
       </c>
-      <c r="U40" s="17">
+      <c r="U40" s="18">
         <v>257.45543181158001</v>
       </c>
     </row>
@@ -4067,7 +3755,7 @@
       <c r="A41" s="8">
         <v>183</v>
       </c>
-      <c r="B41" s="16">
+      <c r="B41" s="17">
         <v>553.554261399604</v>
       </c>
       <c r="C41" s="1">
@@ -4124,7 +3812,7 @@
       <c r="T41" s="1">
         <v>177.74827054257599</v>
       </c>
-      <c r="U41" s="17">
+      <c r="U41" s="18">
         <v>705.71500260275104</v>
       </c>
     </row>
@@ -4132,7 +3820,7 @@
       <c r="A42" s="8">
         <v>184</v>
       </c>
-      <c r="B42" s="16">
+      <c r="B42" s="17">
         <v>79.193458627955906</v>
       </c>
       <c r="C42" s="1">
@@ -4189,7 +3877,7 @@
       <c r="T42" s="1">
         <v>303.778884432604</v>
       </c>
-      <c r="U42" s="17">
+      <c r="U42" s="18">
         <v>545.45820736786197</v>
       </c>
     </row>
@@ -4197,7 +3885,7 @@
       <c r="A43" s="8">
         <v>185</v>
       </c>
-      <c r="B43" s="16">
+      <c r="B43" s="17">
         <v>606.53783934908097</v>
       </c>
       <c r="C43" s="1">
@@ -4254,7 +3942,7 @@
       <c r="T43" s="1">
         <v>59.463187077149797</v>
       </c>
-      <c r="U43" s="17">
+      <c r="U43" s="18">
         <v>991.56610110738302</v>
       </c>
     </row>
@@ -4262,7 +3950,7 @@
       <c r="A44" s="8">
         <v>186</v>
       </c>
-      <c r="B44" s="16">
+      <c r="B44" s="17">
         <v>143.687915100374</v>
       </c>
       <c r="C44" s="1">
@@ -4319,7 +4007,7 @@
       <c r="T44" s="1">
         <v>2.0285637497630802</v>
       </c>
-      <c r="U44" s="17">
+      <c r="U44" s="18">
         <v>1127.2941332509499</v>
       </c>
     </row>
@@ -4327,7 +4015,7 @@
       <c r="A45" s="8">
         <v>187</v>
       </c>
-      <c r="B45" s="16">
+      <c r="B45" s="17">
         <v>206.74614782541099</v>
       </c>
       <c r="C45" s="1">
@@ -4384,7 +4072,7 @@
       <c r="T45" s="1">
         <v>35.456631505136997</v>
       </c>
-      <c r="U45" s="17">
+      <c r="U45" s="18">
         <v>526.16330779288296</v>
       </c>
     </row>
@@ -4392,7 +4080,7 @@
       <c r="A46" s="8">
         <v>188</v>
       </c>
-      <c r="B46" s="16">
+      <c r="B46" s="17">
         <v>192.509997132526</v>
       </c>
       <c r="C46" s="1">
@@ -4449,7 +4137,7 @@
       <c r="T46" s="1">
         <v>16.823790044384499</v>
       </c>
-      <c r="U46" s="17">
+      <c r="U46" s="18">
         <v>380.39405017617298</v>
       </c>
     </row>
@@ -4457,7 +4145,7 @@
       <c r="A47" s="8">
         <v>189</v>
       </c>
-      <c r="B47" s="16">
+      <c r="B47" s="17">
         <v>140.13468462280201</v>
       </c>
       <c r="C47" s="1">
@@ -4514,7 +4202,7 @@
       <c r="T47" s="1">
         <v>45.916005360066102</v>
       </c>
-      <c r="U47" s="17">
+      <c r="U47" s="18">
         <v>1535.9267208839899</v>
       </c>
     </row>
@@ -4522,7 +4210,7 @@
       <c r="A48" s="8">
         <v>190</v>
       </c>
-      <c r="B48" s="16">
+      <c r="B48" s="17">
         <v>66.391325516333495</v>
       </c>
       <c r="C48" s="1">
@@ -4579,7 +4267,7 @@
       <c r="T48" s="1">
         <v>1.1012389917149201E-3</v>
       </c>
-      <c r="U48" s="17">
+      <c r="U48" s="18">
         <v>1597.71429281732</v>
       </c>
     </row>
@@ -4587,7 +4275,7 @@
       <c r="A49" s="8">
         <v>191</v>
       </c>
-      <c r="B49" s="16">
+      <c r="B49" s="17">
         <v>219.87777084738099</v>
       </c>
       <c r="C49" s="1">
@@ -4644,7 +4332,7 @@
       <c r="T49" s="1">
         <v>44.8556395836831</v>
       </c>
-      <c r="U49" s="17">
+      <c r="U49" s="18">
         <v>1195.0624372171401</v>
       </c>
     </row>
@@ -4652,7 +4340,7 @@
       <c r="A50" s="8">
         <v>192</v>
       </c>
-      <c r="B50" s="16">
+      <c r="B50" s="17">
         <v>458.64367072115499</v>
       </c>
       <c r="C50" s="1">
@@ -4709,7 +4397,7 @@
       <c r="T50" s="1">
         <v>216.162545795146</v>
       </c>
-      <c r="U50" s="17">
+      <c r="U50" s="18">
         <v>834.49955926788402</v>
       </c>
     </row>
@@ -4717,7 +4405,7 @@
       <c r="A51" s="8">
         <v>193</v>
       </c>
-      <c r="B51" s="16">
+      <c r="B51" s="17">
         <v>135.961042646609</v>
       </c>
       <c r="C51" s="1">
@@ -4774,7 +4462,7 @@
       <c r="T51" s="1">
         <v>2.8768820439046299</v>
       </c>
-      <c r="U51" s="17">
+      <c r="U51" s="18">
         <v>590.02262068324205</v>
       </c>
     </row>
@@ -4782,7 +4470,7 @@
       <c r="A52" s="8">
         <v>194</v>
       </c>
-      <c r="B52" s="16">
+      <c r="B52" s="17">
         <v>876.08342898460603</v>
       </c>
       <c r="C52" s="1">
@@ -4839,7 +4527,7 @@
       <c r="T52" s="1">
         <v>5.9472010786340403</v>
       </c>
-      <c r="U52" s="17">
+      <c r="U52" s="18">
         <v>665.40927767419703</v>
       </c>
     </row>
@@ -4847,7 +4535,7 @@
       <c r="A53" s="8">
         <v>195</v>
       </c>
-      <c r="B53" s="16">
+      <c r="B53" s="17">
         <v>706.79288394725097</v>
       </c>
       <c r="C53" s="1">
@@ -4904,7 +4592,7 @@
       <c r="T53" s="1">
         <v>69.912906019100902</v>
       </c>
-      <c r="U53" s="17">
+      <c r="U53" s="18">
         <v>611.61139749755796</v>
       </c>
     </row>
@@ -4912,7 +4600,7 @@
       <c r="A54" s="8">
         <v>196</v>
       </c>
-      <c r="B54" s="16">
+      <c r="B54" s="17">
         <v>146.82385576476301</v>
       </c>
       <c r="C54" s="1">
@@ -4969,7 +4657,7 @@
       <c r="T54" s="1">
         <v>22.9959536945486</v>
       </c>
-      <c r="U54" s="17">
+      <c r="U54" s="18">
         <v>732.68075437208495</v>
       </c>
     </row>
@@ -4977,7 +4665,7 @@
       <c r="A55" s="8">
         <v>197</v>
       </c>
-      <c r="B55" s="16">
+      <c r="B55" s="17">
         <v>256.529286321342</v>
       </c>
       <c r="C55" s="1">
@@ -5034,7 +4722,7 @@
       <c r="T55" s="1">
         <v>316.578912105526</v>
       </c>
-      <c r="U55" s="17">
+      <c r="U55" s="18">
         <v>1410.4017930703001</v>
       </c>
     </row>
@@ -5042,7 +4730,7 @@
       <c r="A56" s="8">
         <v>198</v>
       </c>
-      <c r="B56" s="16">
+      <c r="B56" s="17">
         <v>512.33660062065201</v>
       </c>
       <c r="C56" s="1">
@@ -5099,7 +4787,7 @@
       <c r="T56" s="1">
         <v>47.782765332735899</v>
       </c>
-      <c r="U56" s="17">
+      <c r="U56" s="18">
         <v>468.03718900975099</v>
       </c>
     </row>
@@ -5107,7 +4795,7 @@
       <c r="A57" s="8">
         <v>199</v>
       </c>
-      <c r="B57" s="16">
+      <c r="B57" s="17">
         <v>115.893836750322</v>
       </c>
       <c r="C57" s="1">
@@ -5164,7 +4852,7 @@
       <c r="T57" s="1">
         <v>106.35248847724201</v>
       </c>
-      <c r="U57" s="17">
+      <c r="U57" s="18">
         <v>528.46309888795804</v>
       </c>
     </row>
@@ -5172,7 +4860,7 @@
       <c r="A58" s="8">
         <v>200</v>
       </c>
-      <c r="B58" s="16">
+      <c r="B58" s="17">
         <v>90.503403864646899</v>
       </c>
       <c r="C58" s="1">
@@ -5229,7 +4917,7 @@
       <c r="T58" s="1">
         <v>10.4236083908821</v>
       </c>
-      <c r="U58" s="17">
+      <c r="U58" s="18">
         <v>1432.28940448769</v>
       </c>
     </row>
@@ -5237,7 +4925,7 @@
       <c r="A59" s="8">
         <v>201</v>
       </c>
-      <c r="B59" s="16">
+      <c r="B59" s="17">
         <v>409.20323147176202</v>
       </c>
       <c r="C59" s="1">
@@ -5294,7 +4982,7 @@
       <c r="T59" s="1">
         <v>3.6328557081298598</v>
       </c>
-      <c r="U59" s="17">
+      <c r="U59" s="18">
         <v>819.67233489287696</v>
       </c>
     </row>
@@ -5302,7 +4990,7 @@
       <c r="A60" s="8">
         <v>202</v>
       </c>
-      <c r="B60" s="16">
+      <c r="B60" s="17">
         <v>250.11789686444899</v>
       </c>
       <c r="C60" s="1">
@@ -5359,7 +5047,7 @@
       <c r="T60" s="1">
         <v>12.218040300307701</v>
       </c>
-      <c r="U60" s="17">
+      <c r="U60" s="18">
         <v>889.63936951124197</v>
       </c>
     </row>
@@ -5367,7 +5055,7 @@
       <c r="A61" s="8">
         <v>203</v>
       </c>
-      <c r="B61" s="16">
+      <c r="B61" s="17">
         <v>379.91260167840898</v>
       </c>
       <c r="C61" s="1">
@@ -5424,7 +5112,7 @@
       <c r="T61" s="1">
         <v>182.713585574289</v>
       </c>
-      <c r="U61" s="17">
+      <c r="U61" s="18">
         <v>182.65279057514499</v>
       </c>
     </row>
@@ -5432,7 +5120,7 @@
       <c r="A62" s="8">
         <v>204</v>
       </c>
-      <c r="B62" s="16">
+      <c r="B62" s="17">
         <v>158.69319663688299</v>
       </c>
       <c r="C62" s="1">
@@ -5489,7 +5177,7 @@
       <c r="T62" s="1">
         <v>4.6242074076275097</v>
       </c>
-      <c r="U62" s="17">
+      <c r="U62" s="18">
         <v>164.75699604967599</v>
       </c>
     </row>
@@ -5497,7 +5185,7 @@
       <c r="A63" s="8">
         <v>205</v>
       </c>
-      <c r="B63" s="16">
+      <c r="B63" s="17">
         <v>132.31813434068999</v>
       </c>
       <c r="C63" s="1">
@@ -5554,7 +5242,7 @@
       <c r="T63" s="1">
         <v>5.4772229785519997</v>
       </c>
-      <c r="U63" s="17">
+      <c r="U63" s="18">
         <v>184.79997090204799</v>
       </c>
     </row>
@@ -5562,7 +5250,7 @@
       <c r="A64" s="8">
         <v>206</v>
       </c>
-      <c r="B64" s="16">
+      <c r="B64" s="17">
         <v>411.87780426759201</v>
       </c>
       <c r="C64" s="1">
@@ -5619,7 +5307,7 @@
       <c r="T64" s="1">
         <v>19.3466352313817</v>
       </c>
-      <c r="U64" s="17">
+      <c r="U64" s="18">
         <v>3.9368837579132601</v>
       </c>
     </row>
@@ -5627,7 +5315,7 @@
       <c r="A65" s="8">
         <v>207</v>
       </c>
-      <c r="B65" s="16">
+      <c r="B65" s="17">
         <v>170.93400495750299</v>
       </c>
       <c r="C65" s="1">
@@ -5684,7 +5372,7 @@
       <c r="T65" s="1">
         <v>82.285499245175799</v>
       </c>
-      <c r="U65" s="17">
+      <c r="U65" s="18">
         <v>5.8482066818468299</v>
       </c>
     </row>
@@ -5692,7 +5380,7 @@
       <c r="A66" s="8">
         <v>208</v>
       </c>
-      <c r="B66" s="16">
+      <c r="B66" s="17">
         <v>273.908225022078</v>
       </c>
       <c r="C66" s="1">
@@ -5749,7 +5437,7 @@
       <c r="T66" s="1">
         <v>10.203483858574099</v>
       </c>
-      <c r="U66" s="17">
+      <c r="U66" s="18">
         <v>61.537427137248002</v>
       </c>
     </row>
@@ -5757,7 +5445,7 @@
       <c r="A67" s="8">
         <v>209</v>
       </c>
-      <c r="B67" s="16">
+      <c r="B67" s="17">
         <v>7.2737883074081404</v>
       </c>
       <c r="C67" s="1">
@@ -5814,7 +5502,7 @@
       <c r="T67" s="1">
         <v>2.22173174408191</v>
       </c>
-      <c r="U67" s="17">
+      <c r="U67" s="18">
         <v>133.56108922537001</v>
       </c>
     </row>
@@ -5822,7 +5510,7 @@
       <c r="A68" s="8">
         <v>210</v>
       </c>
-      <c r="B68" s="16">
+      <c r="B68" s="17">
         <v>108.252654248734</v>
       </c>
       <c r="C68" s="1">
@@ -5879,7 +5567,7 @@
       <c r="T68" s="1">
         <v>30.5063875477938</v>
       </c>
-      <c r="U68" s="17">
+      <c r="U68" s="18">
         <v>7.6749342933265297E-2</v>
       </c>
     </row>
@@ -5887,7 +5575,7 @@
       <c r="A69" s="8">
         <v>211</v>
       </c>
-      <c r="B69" s="16">
+      <c r="B69" s="17">
         <v>1112.3429767371399</v>
       </c>
       <c r="C69" s="1">
@@ -5944,7 +5632,7 @@
       <c r="T69" s="1">
         <v>367.47994785466699</v>
       </c>
-      <c r="U69" s="17">
+      <c r="U69" s="18">
         <v>117.863826836109</v>
       </c>
     </row>
@@ -5952,7 +5640,7 @@
       <c r="A70" s="8">
         <v>212</v>
       </c>
-      <c r="B70" s="16">
+      <c r="B70" s="17">
         <v>970.26732776182496</v>
       </c>
       <c r="C70" s="1">
@@ -6009,7 +5697,7 @@
       <c r="T70" s="1">
         <v>53.948771496184598</v>
       </c>
-      <c r="U70" s="17">
+      <c r="U70" s="18">
         <v>0.18207338411521901</v>
       </c>
     </row>
@@ -6017,7 +5705,7 @@
       <c r="A71" s="8">
         <v>213</v>
       </c>
-      <c r="B71" s="16">
+      <c r="B71" s="17">
         <v>555.79986479160004</v>
       </c>
       <c r="C71" s="1">
@@ -6074,7 +5762,7 @@
       <c r="T71" s="1">
         <v>1.35082331216443</v>
       </c>
-      <c r="U71" s="17">
+      <c r="U71" s="18">
         <v>12.770629849637199</v>
       </c>
     </row>
@@ -6082,7 +5770,7 @@
       <c r="A72" s="8">
         <v>214</v>
       </c>
-      <c r="B72" s="16">
+      <c r="B72" s="17">
         <v>178.33692308447701</v>
       </c>
       <c r="C72" s="1">
@@ -6139,7 +5827,7 @@
       <c r="T72" s="1">
         <v>23.487445891723599</v>
       </c>
-      <c r="U72" s="17">
+      <c r="U72" s="18">
         <v>15.759718924532599</v>
       </c>
     </row>
@@ -6147,7 +5835,7 @@
       <c r="A73" s="8">
         <v>215</v>
       </c>
-      <c r="B73" s="16">
+      <c r="B73" s="17">
         <v>38.998221785043199</v>
       </c>
       <c r="C73" s="1">
@@ -6204,7 +5892,7 @@
       <c r="T73" s="1">
         <v>5.0326187565348501</v>
       </c>
-      <c r="U73" s="17">
+      <c r="U73" s="18">
         <v>29.446963365578501</v>
       </c>
     </row>
@@ -6212,7 +5900,7 @@
       <c r="A74" s="8">
         <v>216</v>
       </c>
-      <c r="B74" s="16">
+      <c r="B74" s="17">
         <v>9.4297053517937304</v>
       </c>
       <c r="C74" s="1">
@@ -6269,7 +5957,7 @@
       <c r="T74" s="1">
         <v>28.970024446171301</v>
       </c>
-      <c r="U74" s="17">
+      <c r="U74" s="18">
         <v>14.531676679255099</v>
       </c>
     </row>
@@ -6277,7 +5965,7 @@
       <c r="A75" s="8">
         <v>217</v>
       </c>
-      <c r="B75" s="16">
+      <c r="B75" s="17">
         <v>29.9773999867258</v>
       </c>
       <c r="C75" s="1">
@@ -6334,7 +6022,7 @@
       <c r="T75" s="1">
         <v>192.929139543617</v>
       </c>
-      <c r="U75" s="17">
+      <c r="U75" s="18">
         <v>1.64913070426648</v>
       </c>
     </row>
@@ -6342,7 +6030,7 @@
       <c r="A76" s="8">
         <v>218</v>
       </c>
-      <c r="B76" s="16">
+      <c r="B76" s="17">
         <v>119.821509237049</v>
       </c>
       <c r="C76" s="1">
@@ -6399,7 +6087,7 @@
       <c r="T76" s="1">
         <v>100.80511818483301</v>
       </c>
-      <c r="U76" s="17">
+      <c r="U76" s="18">
         <v>80.255084642495007</v>
       </c>
     </row>
@@ -6407,7 +6095,7 @@
       <c r="A77" s="8">
         <v>219</v>
       </c>
-      <c r="B77" s="16">
+      <c r="B77" s="17">
         <v>170.36475152606101</v>
       </c>
       <c r="C77" s="1">
@@ -6464,7 +6152,7 @@
       <c r="T77" s="1">
         <v>214.07415487161799</v>
       </c>
-      <c r="U77" s="17">
+      <c r="U77" s="18">
         <v>7.5757897491478801</v>
       </c>
     </row>
@@ -6472,7 +6160,7 @@
       <c r="A78" s="8">
         <v>220</v>
       </c>
-      <c r="B78" s="16">
+      <c r="B78" s="17">
         <v>93.440763187399497</v>
       </c>
       <c r="C78" s="1">
@@ -6529,7 +6217,7 @@
       <c r="T78" s="1">
         <v>701.58491725843703</v>
       </c>
-      <c r="U78" s="17">
+      <c r="U78" s="18">
         <v>31.177473834540798</v>
       </c>
     </row>
@@ -6537,7 +6225,7 @@
       <c r="A79" s="8">
         <v>221</v>
       </c>
-      <c r="B79" s="16">
+      <c r="B79" s="17">
         <v>73.681464103585895</v>
       </c>
       <c r="C79" s="1">
@@ -6594,7 +6282,7 @@
       <c r="T79" s="1">
         <v>363.800834351091</v>
       </c>
-      <c r="U79" s="17">
+      <c r="U79" s="18">
         <v>24.3235267965769</v>
       </c>
     </row>
@@ -6602,7 +6290,7 @@
       <c r="A80" s="8">
         <v>222</v>
       </c>
-      <c r="B80" s="16">
+      <c r="B80" s="17">
         <v>79.657630047900298</v>
       </c>
       <c r="C80" s="1">
@@ -6659,7 +6347,7 @@
       <c r="T80" s="1">
         <v>0.59392001290748697</v>
       </c>
-      <c r="U80" s="17">
+      <c r="U80" s="18">
         <v>1.4178983074695899</v>
       </c>
     </row>
@@ -6667,7 +6355,7 @@
       <c r="A81" s="8">
         <v>223</v>
       </c>
-      <c r="B81" s="16">
+      <c r="B81" s="17">
         <v>55.223233586291997</v>
       </c>
       <c r="C81" s="1">
@@ -6724,7 +6412,7 @@
       <c r="T81" s="1">
         <v>667.00972379602695</v>
       </c>
-      <c r="U81" s="17">
+      <c r="U81" s="18">
         <v>29.902854177602801</v>
       </c>
     </row>
@@ -6732,7 +6420,7 @@
       <c r="A82" s="8">
         <v>224</v>
       </c>
-      <c r="B82" s="16">
+      <c r="B82" s="17">
         <v>19.111929176956899</v>
       </c>
       <c r="C82" s="1">
@@ -6789,7 +6477,7 @@
       <c r="T82" s="1">
         <v>4.6543940552071197</v>
       </c>
-      <c r="U82" s="17">
+      <c r="U82" s="18">
         <v>42.1497705544284</v>
       </c>
     </row>
@@ -6797,7 +6485,7 @@
       <c r="A83" s="8">
         <v>225</v>
       </c>
-      <c r="B83" s="16">
+      <c r="B83" s="17">
         <v>78.263635835328799</v>
       </c>
       <c r="C83" s="1">
@@ -6854,7 +6542,7 @@
       <c r="T83" s="1">
         <v>42.030828152008297</v>
       </c>
-      <c r="U83" s="17">
+      <c r="U83" s="18">
         <v>41.702931012847401</v>
       </c>
     </row>
@@ -6862,7 +6550,7 @@
       <c r="A84" s="8">
         <v>226</v>
       </c>
-      <c r="B84" s="16">
+      <c r="B84" s="17">
         <v>0.14212280511315101</v>
       </c>
       <c r="C84" s="1">
@@ -6919,7 +6607,7 @@
       <c r="T84" s="1">
         <v>34.829017570365401</v>
       </c>
-      <c r="U84" s="17">
+      <c r="U84" s="18">
         <v>108.35421491501501</v>
       </c>
     </row>
@@ -6927,7 +6615,7 @@
       <c r="A85" s="8">
         <v>227</v>
       </c>
-      <c r="B85" s="16">
+      <c r="B85" s="17">
         <v>150.34171444090799</v>
       </c>
       <c r="C85" s="1">
@@ -6984,7 +6672,7 @@
       <c r="T85" s="1">
         <v>1.6134527894719499</v>
       </c>
-      <c r="U85" s="17">
+      <c r="U85" s="18">
         <v>2.23831622473381</v>
       </c>
     </row>
@@ -6992,7 +6680,7 @@
       <c r="A86" s="8">
         <v>228</v>
       </c>
-      <c r="B86" s="16">
+      <c r="B86" s="17">
         <v>87.732857360266706</v>
       </c>
       <c r="C86" s="1">
@@ -7049,7 +6737,7 @@
       <c r="T86" s="1">
         <v>0.61974830364643196</v>
       </c>
-      <c r="U86" s="17">
+      <c r="U86" s="18">
         <v>281.89691861372597</v>
       </c>
     </row>
@@ -7057,7 +6745,7 @@
       <c r="A87" s="8">
         <v>229</v>
       </c>
-      <c r="B87" s="16">
+      <c r="B87" s="17">
         <v>67.963385965402196</v>
       </c>
       <c r="C87" s="1">
@@ -7114,7 +6802,7 @@
       <c r="T87" s="1">
         <v>135.72739614849201</v>
       </c>
-      <c r="U87" s="17">
+      <c r="U87" s="18">
         <v>69.322088508553193</v>
       </c>
     </row>
@@ -7122,7 +6810,7 @@
       <c r="A88" s="8">
         <v>230</v>
       </c>
-      <c r="B88" s="16">
+      <c r="B88" s="17">
         <v>18.415012003156399</v>
       </c>
       <c r="C88" s="1">
@@ -7179,7 +6867,7 @@
       <c r="T88" s="1">
         <v>709.12557826072805</v>
       </c>
-      <c r="U88" s="17">
+      <c r="U88" s="18">
         <v>49.101877732358503</v>
       </c>
     </row>
@@ -7187,7 +6875,7 @@
       <c r="A89" s="8">
         <v>231</v>
       </c>
-      <c r="B89" s="16">
+      <c r="B89" s="17">
         <v>24.272450629615001</v>
       </c>
       <c r="C89" s="1">
@@ -7244,7 +6932,7 @@
       <c r="T89" s="1">
         <v>491.408540170165</v>
       </c>
-      <c r="U89" s="17">
+      <c r="U89" s="18">
         <v>24.259053798274302</v>
       </c>
     </row>
@@ -7252,7 +6940,7 @@
       <c r="A90" s="8">
         <v>232</v>
       </c>
-      <c r="B90" s="16">
+      <c r="B90" s="17">
         <v>50.292785992011602</v>
       </c>
       <c r="C90" s="1">
@@ -7309,7 +6997,7 @@
       <c r="T90" s="1">
         <v>351.93895470380602</v>
       </c>
-      <c r="U90" s="17">
+      <c r="U90" s="18">
         <v>130.256952300959</v>
       </c>
     </row>
@@ -7317,7 +7005,7 @@
       <c r="A91" s="8">
         <v>233</v>
       </c>
-      <c r="B91" s="16">
+      <c r="B91" s="17">
         <v>91.2899255657737</v>
       </c>
       <c r="C91" s="1">
@@ -7374,7 +7062,7 @@
       <c r="T91" s="1">
         <v>304.91298708119598</v>
       </c>
-      <c r="U91" s="17">
+      <c r="U91" s="18">
         <v>1.1595699148341601</v>
       </c>
     </row>
@@ -7382,7 +7070,7 @@
       <c r="A92" s="8">
         <v>234</v>
       </c>
-      <c r="B92" s="16">
+      <c r="B92" s="17">
         <v>281.71669568869902</v>
       </c>
       <c r="C92" s="1">
@@ -7439,7 +7127,7 @@
       <c r="T92" s="1">
         <v>421.21239619289099</v>
       </c>
-      <c r="U92" s="17">
+      <c r="U92" s="18">
         <v>26.186667698036199</v>
       </c>
     </row>
@@ -7447,7 +7135,7 @@
       <c r="A93" s="8">
         <v>235</v>
       </c>
-      <c r="B93" s="16">
+      <c r="B93" s="17">
         <v>119.060523972398</v>
       </c>
       <c r="C93" s="1">
@@ -7504,7 +7192,7 @@
       <c r="T93" s="1">
         <v>616.43597767114602</v>
       </c>
-      <c r="U93" s="17">
+      <c r="U93" s="18">
         <v>22.746480296591901</v>
       </c>
     </row>
@@ -7512,7 +7200,7 @@
       <c r="A94" s="8">
         <v>236</v>
       </c>
-      <c r="B94" s="16">
+      <c r="B94" s="17">
         <v>46.580849615791202</v>
       </c>
       <c r="C94" s="1">
@@ -7569,7 +7257,7 @@
       <c r="T94" s="1">
         <v>5.5026856923514202</v>
       </c>
-      <c r="U94" s="17">
+      <c r="U94" s="18">
         <v>88.034071649511901</v>
       </c>
     </row>
@@ -7577,7 +7265,7 @@
       <c r="A95" s="8">
         <v>237</v>
       </c>
-      <c r="B95" s="16">
+      <c r="B95" s="17">
         <v>2.33338304715538</v>
       </c>
       <c r="C95" s="1">
@@ -7634,7 +7322,7 @@
       <c r="T95" s="1">
         <v>168.04788835444199</v>
       </c>
-      <c r="U95" s="17">
+      <c r="U95" s="18">
         <v>115.089864701694</v>
       </c>
     </row>
@@ -7642,7 +7330,7 @@
       <c r="A96" s="8">
         <v>238</v>
       </c>
-      <c r="B96" s="16">
+      <c r="B96" s="17">
         <v>57.447595228694396</v>
       </c>
       <c r="C96" s="1">
@@ -7699,15 +7387,15 @@
       <c r="T96" s="1">
         <v>91.722722564084705</v>
       </c>
-      <c r="U96" s="17">
+      <c r="U96" s="18">
         <v>366.20461894583599</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <v>239</v>
       </c>
-      <c r="B97" s="16">
+      <c r="B97" s="17">
         <v>68.948057665002594</v>
       </c>
       <c r="C97" s="1">
@@ -7764,15 +7452,15 @@
       <c r="T97" s="1">
         <v>240.78988693338701</v>
       </c>
-      <c r="U97" s="17">
+      <c r="U97" s="18">
         <v>942.46667622685595</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <v>240</v>
       </c>
-      <c r="B98" s="16">
+      <c r="B98" s="17">
         <v>24.316741162659302</v>
       </c>
       <c r="C98" s="1">
@@ -7829,15 +7517,15 @@
       <c r="T98" s="1">
         <v>324.70628124349201</v>
       </c>
-      <c r="U98" s="17">
+      <c r="U98" s="18">
         <v>363.31006732297698</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <v>241</v>
       </c>
-      <c r="B99" s="16">
+      <c r="B99" s="17">
         <v>188.18669611534099</v>
       </c>
       <c r="C99" s="1">
@@ -7894,15 +7582,15 @@
       <c r="T99" s="1">
         <v>532.76483298703499</v>
       </c>
-      <c r="U99" s="17">
+      <c r="U99" s="18">
         <v>1176.4931637027</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
         <v>242</v>
       </c>
-      <c r="B100" s="16">
+      <c r="B100" s="17">
         <v>27.5924213809961</v>
       </c>
       <c r="C100" s="1">
@@ -7959,15 +7647,15 @@
       <c r="T100" s="1">
         <v>994.79623194062901</v>
       </c>
-      <c r="U100" s="17">
+      <c r="U100" s="18">
         <v>456.69596005868101</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" s="8">
         <v>243</v>
       </c>
-      <c r="B101" s="16">
+      <c r="B101" s="17">
         <v>12.7889936337923</v>
       </c>
       <c r="C101" s="1">
@@ -8024,15 +7712,15 @@
       <c r="T101" s="1">
         <v>285.50418490691197</v>
       </c>
-      <c r="U101" s="17">
+      <c r="U101" s="18">
         <v>1249.36606584944</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102" s="8">
         <v>244</v>
       </c>
-      <c r="B102" s="16">
+      <c r="B102" s="17">
         <v>108.197521592524</v>
       </c>
       <c r="C102" s="1">
@@ -8089,15 +7777,15 @@
       <c r="T102" s="1">
         <v>355.13078026417702</v>
       </c>
-      <c r="U102" s="17">
+      <c r="U102" s="18">
         <v>664.35335575985096</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <v>245</v>
       </c>
-      <c r="B103" s="16">
+      <c r="B103" s="17">
         <v>3.23553750804935</v>
       </c>
       <c r="C103" s="1">
@@ -8154,15 +7842,15 @@
       <c r="T103" s="1">
         <v>4.2505568145190296</v>
       </c>
-      <c r="U103" s="17">
+      <c r="U103" s="18">
         <v>654.30058124727896</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" s="8">
         <v>246</v>
       </c>
-      <c r="B104" s="16">
+      <c r="B104" s="17">
         <v>89.309115617501604</v>
       </c>
       <c r="C104" s="1">
@@ -8219,15 +7907,15 @@
       <c r="T104" s="1">
         <v>335.315644296892</v>
       </c>
-      <c r="U104" s="17">
+      <c r="U104" s="18">
         <v>400.57377526540103</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="9">
         <v>247</v>
       </c>
-      <c r="B105" s="19">
+      <c r="B105" s="20">
         <v>3.07916420882162</v>
       </c>
       <c r="C105" s="10">
@@ -8284,12 +7972,12 @@
       <c r="T105" s="10">
         <v>448.07857631114899</v>
       </c>
-      <c r="U105" s="20">
+      <c r="U105" s="21">
         <v>711.77358159756602</v>
       </c>
     </row>
-    <row r="106" spans="1:23" s="38" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="22" t="s">
+    <row r="106" spans="1:21" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B106" s="11">
@@ -8349,736 +8037,76 @@
       <c r="T106" s="12">
         <v>17805.790822712399</v>
       </c>
-      <c r="U106" s="21">
+      <c r="U106" s="22">
         <v>31061.5810070349</v>
       </c>
     </row>
-    <row r="107" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="29" t="s">
+    <row r="107" spans="1:21" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B107" s="39">
+      <c r="B107" s="23">
         <v>164.99749695003501</v>
       </c>
-      <c r="C107" s="40">
+      <c r="C107" s="13">
         <v>112.228027215559</v>
       </c>
-      <c r="D107" s="40">
+      <c r="D107" s="13">
         <v>80.5989667625457</v>
       </c>
-      <c r="E107" s="40">
+      <c r="E107" s="13">
         <v>400.68527566727101</v>
       </c>
-      <c r="F107" s="40">
+      <c r="F107" s="13">
         <v>55.234398369686502</v>
       </c>
-      <c r="G107" s="40">
+      <c r="G107" s="13">
         <v>198.63362964283101</v>
       </c>
-      <c r="H107" s="40">
+      <c r="H107" s="13">
         <v>123.299678772796</v>
       </c>
-      <c r="I107" s="40">
+      <c r="I107" s="13">
         <v>117.36799843211899</v>
       </c>
-      <c r="J107" s="40">
+      <c r="J107" s="13">
         <v>357.996136772189</v>
       </c>
-      <c r="K107" s="40">
+      <c r="K107" s="13">
         <v>127.979862218031</v>
       </c>
-      <c r="L107" s="40">
+      <c r="L107" s="13">
         <v>178.96813555334001</v>
       </c>
-      <c r="M107" s="40">
+      <c r="M107" s="13">
         <v>75.727682536596603</v>
       </c>
-      <c r="N107" s="40">
+      <c r="N107" s="13">
         <v>69.764207250338103</v>
       </c>
-      <c r="O107" s="40">
+      <c r="O107" s="13">
         <v>40.384816501307</v>
       </c>
-      <c r="P107" s="40">
+      <c r="P107" s="13">
         <v>40.384816501305998</v>
       </c>
-      <c r="Q107" s="40">
+      <c r="Q107" s="13">
         <v>308.42922264843003</v>
       </c>
-      <c r="R107" s="40">
+      <c r="R107" s="13">
         <v>103.87834323926501</v>
       </c>
-      <c r="S107" s="40">
+      <c r="S107" s="13">
         <v>270.377835037892</v>
       </c>
-      <c r="T107" s="40">
+      <c r="T107" s="13">
         <v>171.209527141466</v>
       </c>
-      <c r="U107" s="41">
+      <c r="U107" s="24">
         <v>298.66904814456598</v>
       </c>
     </row>
-    <row r="108" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="30">
-        <v>3</v>
-      </c>
-      <c r="B108" s="31">
-        <v>37358.745517000003</v>
-      </c>
-      <c r="C108" s="31">
-        <v>28148.977627699998</v>
-      </c>
-      <c r="D108" s="31">
-        <v>45057.311510799998</v>
-      </c>
-      <c r="E108" s="31">
-        <v>23755.507646099999</v>
-      </c>
-      <c r="F108" s="31">
-        <v>3762.4906298000001</v>
-      </c>
-      <c r="G108" s="31">
-        <v>28107.904547300001</v>
-      </c>
-      <c r="H108" s="31">
-        <v>12266.047646000001</v>
-      </c>
-      <c r="I108" s="31">
-        <v>3179280.01021</v>
-      </c>
-      <c r="J108" s="31">
-        <v>34955.912040800002</v>
-      </c>
-      <c r="K108" s="31">
-        <v>30527.8521048</v>
-      </c>
-      <c r="L108" s="31">
-        <v>26964.3784586</v>
-      </c>
-      <c r="M108" s="31">
-        <v>14109.9270089</v>
-      </c>
-      <c r="N108" s="31">
-        <v>7532859128</v>
-      </c>
-      <c r="O108" s="31">
-        <v>2440.8958397900001</v>
-      </c>
-      <c r="P108" s="31">
-        <v>38112.229176100001</v>
-      </c>
-      <c r="Q108" s="31">
-        <v>161879.476502</v>
-      </c>
-      <c r="R108" s="31">
-        <v>29408.958609900001</v>
-      </c>
-      <c r="S108" s="31">
-        <v>166662.00752799999</v>
-      </c>
-      <c r="T108" s="31">
-        <v>49933.076868999997</v>
-      </c>
-      <c r="U108" s="31">
-        <v>89483.030446899997</v>
-      </c>
-    </row>
-    <row r="109" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="30"/>
-      <c r="B109" s="31">
-        <v>359.21870689399998</v>
-      </c>
-      <c r="C109" s="31">
-        <v>270.663246421</v>
-      </c>
-      <c r="D109" s="31">
-        <v>433.24337991099998</v>
-      </c>
-      <c r="E109" s="32">
-        <v>228.41834275100001</v>
-      </c>
-      <c r="F109" s="32">
-        <v>36.177794517300001</v>
-      </c>
-      <c r="G109" s="31">
-        <v>270.268312955</v>
-      </c>
-      <c r="H109" s="32">
-        <v>117.942765827</v>
-      </c>
-      <c r="I109" s="31">
-        <v>30570.000098199998</v>
-      </c>
-      <c r="J109" s="32">
-        <v>336.11453885399999</v>
-      </c>
-      <c r="K109" s="31">
-        <v>293.53703946899998</v>
-      </c>
-      <c r="L109" s="31">
-        <v>259.27286979399997</v>
-      </c>
-      <c r="M109" s="31">
-        <v>135.67237508599999</v>
-      </c>
-      <c r="N109" s="31">
-        <v>72431337.769199997</v>
-      </c>
-      <c r="O109" s="32">
-        <v>23.470152305700001</v>
-      </c>
-      <c r="P109" s="31">
-        <v>366.463742078</v>
-      </c>
-      <c r="Q109" s="31">
-        <v>1556.5334279000001</v>
-      </c>
-      <c r="R109" s="31">
-        <v>282.77844817300002</v>
-      </c>
-      <c r="S109" s="31">
-        <v>1602.5193031599999</v>
-      </c>
-      <c r="T109" s="31">
-        <v>480.125739125</v>
-      </c>
-      <c r="U109" s="31">
-        <v>860.41375429699997</v>
-      </c>
-      <c r="V109" s="26">
-        <f>SUM(B109:U109)</f>
-        <v>72469820.603237718</v>
-      </c>
-      <c r="W109" s="26">
-        <f>V109/20</f>
-        <v>3623491.030161886</v>
-      </c>
-    </row>
-    <row r="110" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="48">
-        <v>4</v>
-      </c>
-      <c r="B110" s="49">
-        <v>27460.4418931</v>
-      </c>
-      <c r="C110" s="49">
-        <v>19370.307719699998</v>
-      </c>
-      <c r="D110" s="49">
-        <v>14219.011034900001</v>
-      </c>
-      <c r="E110" s="49">
-        <v>24698.834751499999</v>
-      </c>
-      <c r="F110" s="49">
-        <v>6811.3987406400001</v>
-      </c>
-      <c r="G110" s="49">
-        <v>39549.776564899999</v>
-      </c>
-      <c r="H110" s="49">
-        <v>12715.3132042</v>
-      </c>
-      <c r="I110" s="49">
-        <v>34995.379671399998</v>
-      </c>
-      <c r="J110" s="49">
-        <v>39289.896746099999</v>
-      </c>
-      <c r="K110" s="49">
-        <v>21265.686675500001</v>
-      </c>
-      <c r="L110" s="49">
-        <v>34756.449921699998</v>
-      </c>
-      <c r="M110" s="49">
-        <v>14157.8313361</v>
-      </c>
-      <c r="N110" s="49">
-        <v>23834.417611100002</v>
-      </c>
-      <c r="O110" s="49">
-        <v>2267.8282804700002</v>
-      </c>
-      <c r="P110" s="49">
-        <v>3596.8106818199999</v>
-      </c>
-      <c r="Q110" s="49">
-        <v>69625.387884399999</v>
-      </c>
-      <c r="R110" s="49">
-        <v>26464.8856705</v>
-      </c>
-      <c r="S110" s="49">
-        <v>12180.917567300001</v>
-      </c>
-      <c r="T110" s="49">
-        <v>22952.030774499999</v>
-      </c>
-      <c r="U110" s="49">
-        <v>118309.648812</v>
-      </c>
-      <c r="V110" s="50"/>
-    </row>
-    <row r="111" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="48"/>
-      <c r="B111" s="49">
-        <v>264.042710511</v>
-      </c>
-      <c r="C111" s="49">
-        <v>186.25295884400001</v>
-      </c>
-      <c r="D111" s="49">
-        <v>136.72125995100001</v>
-      </c>
-      <c r="E111" s="49">
-        <v>237.48879568699999</v>
-      </c>
-      <c r="F111" s="49">
-        <v>65.494218660000001</v>
-      </c>
-      <c r="G111" s="49">
-        <v>380.286313124</v>
-      </c>
-      <c r="H111" s="51">
-        <v>122.262626963</v>
-      </c>
-      <c r="I111" s="49">
-        <v>336.49403530199999</v>
-      </c>
-      <c r="J111" s="49">
-        <v>377.78746871300001</v>
-      </c>
-      <c r="K111" s="49">
-        <v>204.47775649499999</v>
-      </c>
-      <c r="L111" s="49">
-        <v>334.19663386299999</v>
-      </c>
-      <c r="M111" s="49">
-        <v>136.13299361700001</v>
-      </c>
-      <c r="N111" s="49">
-        <v>229.17709241399999</v>
-      </c>
-      <c r="O111" s="51">
-        <v>21.806041158300001</v>
-      </c>
-      <c r="P111" s="51">
-        <v>34.584718094400003</v>
-      </c>
-      <c r="Q111" s="49">
-        <v>669.47488350399999</v>
-      </c>
-      <c r="R111" s="49">
-        <v>254.47005452400001</v>
-      </c>
-      <c r="S111" s="51">
-        <v>117.12420737799999</v>
-      </c>
-      <c r="T111" s="49">
-        <v>220.692603601</v>
-      </c>
-      <c r="U111" s="49">
-        <v>1137.5927770400001</v>
-      </c>
-      <c r="V111" s="50">
-        <f t="shared" ref="V110:V115" si="0">SUM(B111:U111)</f>
-        <v>5466.5601494437005</v>
-      </c>
-      <c r="W111" s="27">
-        <f>V111/20</f>
-        <v>273.32800747218505</v>
-      </c>
-    </row>
-    <row r="112" spans="1:23" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="33">
-        <v>5</v>
-      </c>
-      <c r="B112" s="34">
-        <v>19455.528460900001</v>
-      </c>
-      <c r="C112" s="34">
-        <v>36831.366647199997</v>
-      </c>
-      <c r="D112" s="34">
-        <v>16619.481868300001</v>
-      </c>
-      <c r="E112" s="34">
-        <v>31816.254222399999</v>
-      </c>
-      <c r="F112" s="34">
-        <v>3408.8993179600002</v>
-      </c>
-      <c r="G112" s="34">
-        <v>29848.338228199998</v>
-      </c>
-      <c r="H112" s="34">
-        <v>14570.7416512</v>
-      </c>
-      <c r="I112" s="34">
-        <v>46974.141749399998</v>
-      </c>
-      <c r="J112" s="34">
-        <v>47855.750460099996</v>
-      </c>
-      <c r="K112" s="34">
-        <v>35328.118900300004</v>
-      </c>
-      <c r="L112" s="34">
-        <v>17651.048396599999</v>
-      </c>
-      <c r="M112" s="34">
-        <v>15563.788933600001</v>
-      </c>
-      <c r="N112" s="34">
-        <v>22038.882111200001</v>
-      </c>
-      <c r="O112" s="34">
-        <v>1670.33962572</v>
-      </c>
-      <c r="P112" s="34">
-        <v>5799.1805206700001</v>
-      </c>
-      <c r="Q112" s="34">
-        <v>19756.070047900001</v>
-      </c>
-      <c r="R112" s="34">
-        <v>17790.9325245</v>
-      </c>
-      <c r="S112" s="34">
-        <v>16087.749815900001</v>
-      </c>
-      <c r="T112" s="34">
-        <v>19574.1229958</v>
-      </c>
-      <c r="U112" s="34">
-        <v>78841.273471099994</v>
-      </c>
-      <c r="V112" s="45"/>
-    </row>
-    <row r="113" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="33"/>
-      <c r="B113" s="34">
-        <v>187.072389047</v>
-      </c>
-      <c r="C113" s="34">
-        <v>354.14775622299999</v>
-      </c>
-      <c r="D113" s="34">
-        <v>159.80271027200001</v>
-      </c>
-      <c r="E113" s="34">
-        <v>305.92552136900002</v>
-      </c>
-      <c r="F113" s="35">
-        <v>32.777878057300001</v>
-      </c>
-      <c r="G113" s="34">
-        <v>287.00325219400003</v>
-      </c>
-      <c r="H113" s="34">
-        <v>140.10328510799999</v>
-      </c>
-      <c r="I113" s="34">
-        <v>451.674439898</v>
-      </c>
-      <c r="J113" s="34">
-        <v>460.15144673200001</v>
-      </c>
-      <c r="K113" s="34">
-        <v>339.69345096400002</v>
-      </c>
-      <c r="L113" s="35">
-        <v>169.72161919800001</v>
-      </c>
-      <c r="M113" s="34">
-        <v>149.651816669</v>
-      </c>
-      <c r="N113" s="34">
-        <v>211.912327992</v>
-      </c>
-      <c r="O113" s="35">
-        <v>16.060957939600002</v>
-      </c>
-      <c r="P113" s="34">
-        <v>55.761351160300002</v>
-      </c>
-      <c r="Q113" s="35">
-        <v>189.962211999</v>
-      </c>
-      <c r="R113" s="34">
-        <v>171.066658889</v>
-      </c>
-      <c r="S113" s="35">
-        <v>154.68990207600001</v>
-      </c>
-      <c r="T113" s="34">
-        <v>188.21272111299999</v>
-      </c>
-      <c r="U113" s="34">
-        <v>758.08916799099995</v>
-      </c>
-      <c r="V113" s="45">
-        <f t="shared" si="0"/>
-        <v>4783.4808648911994</v>
-      </c>
-      <c r="W113" s="25">
-        <f>V113/20</f>
-        <v>239.17404324455998</v>
-      </c>
-    </row>
-    <row r="114" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="36">
-        <v>6</v>
-      </c>
-      <c r="B114" s="37">
-        <v>26921.8215098</v>
-      </c>
-      <c r="C114" s="37">
-        <v>28677.640186299999</v>
-      </c>
-      <c r="D114" s="37">
-        <v>24861.734785199998</v>
-      </c>
-      <c r="E114" s="37">
-        <v>110776.71392900001</v>
-      </c>
-      <c r="F114" s="37">
-        <v>2993.75698371</v>
-      </c>
-      <c r="G114" s="37">
-        <v>29940.7345661</v>
-      </c>
-      <c r="H114" s="37">
-        <v>8256.1330484600003</v>
-      </c>
-      <c r="I114" s="37">
-        <v>42134.900773900001</v>
-      </c>
-      <c r="J114" s="37">
-        <v>41146.3352199</v>
-      </c>
-      <c r="K114" s="37">
-        <v>35497.699881400004</v>
-      </c>
-      <c r="L114" s="37">
-        <v>25982.719393399999</v>
-      </c>
-      <c r="M114" s="37">
-        <v>8758.6512665200007</v>
-      </c>
-      <c r="N114" s="37">
-        <v>15294.252718</v>
-      </c>
-      <c r="O114" s="37">
-        <v>115899.42303599999</v>
-      </c>
-      <c r="P114" s="37">
-        <v>2591.3519432100002</v>
-      </c>
-      <c r="Q114" s="37">
-        <v>35497.114962899999</v>
-      </c>
-      <c r="R114" s="37">
-        <v>11810.5707791</v>
-      </c>
-      <c r="S114" s="37">
-        <v>33886.1813502</v>
-      </c>
-      <c r="T114" s="37">
-        <v>23039.208666800001</v>
-      </c>
-      <c r="U114" s="37">
-        <v>348347.20829699998</v>
-      </c>
-      <c r="V114" s="47"/>
-    </row>
-    <row r="115" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="36"/>
-      <c r="B115" s="52">
-        <v>258.86366836299999</v>
-      </c>
-      <c r="C115" s="52">
-        <v>275.74654025299998</v>
-      </c>
-      <c r="D115" s="52">
-        <v>239.05514216500001</v>
-      </c>
-      <c r="E115" s="52">
-        <v>1065.16071085</v>
-      </c>
-      <c r="F115" s="53">
-        <v>28.786124843300001</v>
-      </c>
-      <c r="G115" s="52">
-        <v>287.89167852100002</v>
-      </c>
-      <c r="H115" s="53">
-        <v>79.385894696700007</v>
-      </c>
-      <c r="I115" s="52">
-        <v>405.14327667200001</v>
-      </c>
-      <c r="J115" s="52">
-        <v>395.63783865300002</v>
-      </c>
-      <c r="K115" s="52">
-        <v>341.32403732099999</v>
-      </c>
-      <c r="L115" s="52">
-        <v>249.833840321</v>
-      </c>
-      <c r="M115" s="52">
-        <v>84.2178006396</v>
-      </c>
-      <c r="N115" s="52">
-        <v>147.06012228899999</v>
-      </c>
-      <c r="O115" s="52">
-        <v>1114.4175292</v>
-      </c>
-      <c r="P115" s="53">
-        <v>24.916845607799999</v>
-      </c>
-      <c r="Q115" s="52">
-        <v>341.318413104</v>
-      </c>
-      <c r="R115" s="52">
-        <v>113.56318056800001</v>
-      </c>
-      <c r="S115" s="52">
-        <v>325.82866682899999</v>
-      </c>
-      <c r="T115" s="52">
-        <v>221.53085256599999</v>
-      </c>
-      <c r="U115" s="52">
-        <v>3349.4923874699998</v>
-      </c>
-      <c r="V115" s="47">
-        <f t="shared" si="0"/>
-        <v>9349.1745509323991</v>
-      </c>
-      <c r="W115" s="28">
-        <f>V115/20</f>
-        <v>467.45872754661997</v>
-      </c>
-    </row>
-    <row r="116" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="43">
-        <v>7</v>
-      </c>
-      <c r="B116" s="44">
-        <v>20274.647340799998</v>
-      </c>
-    </row>
-    <row r="117" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="43"/>
-      <c r="B117" s="44">
-        <v>194.94853212300001</v>
-      </c>
-    </row>
-    <row r="118" spans="1:23" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="54">
-        <v>8</v>
-      </c>
-      <c r="B118" s="55">
-        <v>23855.423083400001</v>
-      </c>
-    </row>
-    <row r="119" spans="1:23" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="54"/>
-      <c r="B119" s="55">
-        <v>229.37906810999999</v>
-      </c>
-    </row>
-    <row r="120" spans="1:23" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="57">
-        <v>9</v>
-      </c>
-      <c r="B120" s="58">
-        <v>21923.905306600001</v>
-      </c>
-    </row>
-    <row r="121" spans="1:23" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="57"/>
-      <c r="B121" s="58">
-        <v>210.80678179500001</v>
-      </c>
-    </row>
-    <row r="122" spans="1:23" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="60">
-        <v>10</v>
-      </c>
-      <c r="B122" s="46">
-        <v>25974.9545082</v>
-      </c>
-    </row>
-    <row r="123" spans="1:23" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="61"/>
-      <c r="B123" s="46">
-        <v>249.75917796300001</v>
-      </c>
-    </row>
-    <row r="124" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="62">
-        <v>10</v>
-      </c>
-      <c r="B124" s="59">
-        <v>48199.039138200002</v>
-      </c>
-    </row>
-    <row r="125" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="63"/>
-      <c r="B125" s="59">
-        <v>463.45229940500002</v>
-      </c>
-    </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A126" s="42">
-        <v>11</v>
-      </c>
-      <c r="B126">
-        <v>23117.037772</v>
-      </c>
-    </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A127" s="56"/>
-      <c r="B127">
-        <v>222.27920934599999</v>
-      </c>
-    </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A128" s="23">
-        <v>12</v>
-      </c>
-      <c r="B128">
-        <v>22660.990475899998</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="23"/>
-      <c r="B129">
-        <v>217.89413919099999</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A124:A125"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="A110:A111"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A119"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>